<commit_message>
updates to Additional Reports: Seeded Acres
</commit_message>
<xml_diff>
--- a/UploadedFiles/SeededAcres.xlsx
+++ b/UploadedFiles/SeededAcres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4250" uniqueCount="43">
   <si>
     <t>FiscalYear</t>
   </si>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2161" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2120" totalsRowShown="0">
   <tableColumns count="12">
     <tableColumn id="1" name="FiscalYear"/>
     <tableColumn id="2" name="FiscalPeriod"/>
@@ -495,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2161"/>
+  <dimension ref="A1:L2120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -81074,1564 +81074,6 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2121">
-        <v>2017</v>
-      </c>
-      <c r="B2121">
-        <v>3</v>
-      </c>
-      <c r="C2121" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2121" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2121">
-        <v>200</v>
-      </c>
-      <c r="F2121">
-        <v>200</v>
-      </c>
-      <c r="G2121">
-        <v>200</v>
-      </c>
-      <c r="H2121">
-        <v>200</v>
-      </c>
-      <c r="I2121">
-        <v>958</v>
-      </c>
-      <c r="J2121">
-        <v>958</v>
-      </c>
-      <c r="K2121">
-        <v>1045</v>
-      </c>
-      <c r="L2121">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="2122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2122">
-        <v>2017</v>
-      </c>
-      <c r="B2122">
-        <v>3</v>
-      </c>
-      <c r="C2122" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2122" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2122">
-        <v>-48</v>
-      </c>
-      <c r="F2122">
-        <v>-144</v>
-      </c>
-      <c r="G2122">
-        <v>749</v>
-      </c>
-      <c r="H2122">
-        <v>2247</v>
-      </c>
-      <c r="I2122">
-        <v>7</v>
-      </c>
-      <c r="J2122">
-        <v>21</v>
-      </c>
-      <c r="K2122">
-        <v>536</v>
-      </c>
-      <c r="L2122">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="2123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2123">
-        <v>2017</v>
-      </c>
-      <c r="B2123">
-        <v>3</v>
-      </c>
-      <c r="C2123" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2123" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2123">
-        <v>0</v>
-      </c>
-      <c r="F2123">
-        <v>0</v>
-      </c>
-      <c r="G2123">
-        <v>2</v>
-      </c>
-      <c r="H2123">
-        <v>34</v>
-      </c>
-      <c r="I2123">
-        <v>1</v>
-      </c>
-      <c r="J2123">
-        <v>17</v>
-      </c>
-      <c r="K2123">
-        <v>37</v>
-      </c>
-      <c r="L2123">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="2124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2124">
-        <v>2017</v>
-      </c>
-      <c r="B2124">
-        <v>3</v>
-      </c>
-      <c r="C2124" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2124" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2124">
-        <v>5</v>
-      </c>
-      <c r="F2124">
-        <v>55</v>
-      </c>
-      <c r="G2124">
-        <v>20</v>
-      </c>
-      <c r="H2124">
-        <v>220</v>
-      </c>
-      <c r="I2124">
-        <v>12</v>
-      </c>
-      <c r="J2124">
-        <v>132</v>
-      </c>
-      <c r="K2124">
-        <v>38</v>
-      </c>
-      <c r="L2124">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="2125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2125">
-        <v>2017</v>
-      </c>
-      <c r="B2125">
-        <v>3</v>
-      </c>
-      <c r="C2125" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2125" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2125">
-        <v>42</v>
-      </c>
-      <c r="F2125">
-        <v>714</v>
-      </c>
-      <c r="G2125">
-        <v>42</v>
-      </c>
-      <c r="H2125">
-        <v>714</v>
-      </c>
-      <c r="I2125">
-        <v>0</v>
-      </c>
-      <c r="J2125">
-        <v>0</v>
-      </c>
-      <c r="K2125">
-        <v>0</v>
-      </c>
-      <c r="L2125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2126">
-        <v>2017</v>
-      </c>
-      <c r="B2126">
-        <v>3</v>
-      </c>
-      <c r="C2126" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2126" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2126">
-        <v>440</v>
-      </c>
-      <c r="F2126">
-        <v>440</v>
-      </c>
-      <c r="G2126">
-        <v>440</v>
-      </c>
-      <c r="H2126">
-        <v>440</v>
-      </c>
-      <c r="I2126">
-        <v>0</v>
-      </c>
-      <c r="J2126">
-        <v>0</v>
-      </c>
-      <c r="K2126">
-        <v>0</v>
-      </c>
-      <c r="L2126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2127">
-        <v>2017</v>
-      </c>
-      <c r="B2127">
-        <v>3</v>
-      </c>
-      <c r="C2127" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2127" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2127">
-        <v>0</v>
-      </c>
-      <c r="F2127">
-        <v>0</v>
-      </c>
-      <c r="G2127">
-        <v>227</v>
-      </c>
-      <c r="H2127">
-        <v>681</v>
-      </c>
-      <c r="I2127">
-        <v>72</v>
-      </c>
-      <c r="J2127">
-        <v>216</v>
-      </c>
-      <c r="K2127">
-        <v>200</v>
-      </c>
-      <c r="L2127">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="2128" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2128">
-        <v>2017</v>
-      </c>
-      <c r="B2128">
-        <v>3</v>
-      </c>
-      <c r="C2128" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2128" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2128">
-        <v>0</v>
-      </c>
-      <c r="F2128">
-        <v>0</v>
-      </c>
-      <c r="G2128">
-        <v>0</v>
-      </c>
-      <c r="H2128">
-        <v>0</v>
-      </c>
-      <c r="I2128">
-        <v>-1</v>
-      </c>
-      <c r="J2128">
-        <v>-17</v>
-      </c>
-      <c r="K2128">
-        <v>3</v>
-      </c>
-      <c r="L2128">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2129" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2129">
-        <v>2017</v>
-      </c>
-      <c r="B2129">
-        <v>3</v>
-      </c>
-      <c r="C2129" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2129" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2129">
-        <v>0</v>
-      </c>
-      <c r="F2129">
-        <v>0</v>
-      </c>
-      <c r="G2129">
-        <v>1</v>
-      </c>
-      <c r="H2129">
-        <v>11</v>
-      </c>
-      <c r="I2129">
-        <v>0</v>
-      </c>
-      <c r="J2129">
-        <v>0</v>
-      </c>
-      <c r="K2129">
-        <v>2</v>
-      </c>
-      <c r="L2129">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2130">
-        <v>2017</v>
-      </c>
-      <c r="B2130">
-        <v>3</v>
-      </c>
-      <c r="C2130" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2130" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2130">
-        <v>0</v>
-      </c>
-      <c r="F2130">
-        <v>0</v>
-      </c>
-      <c r="G2130">
-        <v>69</v>
-      </c>
-      <c r="H2130">
-        <v>207</v>
-      </c>
-      <c r="I2130">
-        <v>0</v>
-      </c>
-      <c r="J2130">
-        <v>0</v>
-      </c>
-      <c r="K2130">
-        <v>94</v>
-      </c>
-      <c r="L2130">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="2131" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2131">
-        <v>2017</v>
-      </c>
-      <c r="B2131">
-        <v>3</v>
-      </c>
-      <c r="C2131" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2131" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2131">
-        <v>0</v>
-      </c>
-      <c r="F2131">
-        <v>0</v>
-      </c>
-      <c r="G2131">
-        <v>6</v>
-      </c>
-      <c r="H2131">
-        <v>102</v>
-      </c>
-      <c r="I2131">
-        <v>0</v>
-      </c>
-      <c r="J2131">
-        <v>0</v>
-      </c>
-      <c r="K2131">
-        <v>0</v>
-      </c>
-      <c r="L2131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2132">
-        <v>2017</v>
-      </c>
-      <c r="B2132">
-        <v>3</v>
-      </c>
-      <c r="C2132" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2132" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2132">
-        <v>1</v>
-      </c>
-      <c r="F2132">
-        <v>11</v>
-      </c>
-      <c r="G2132">
-        <v>5</v>
-      </c>
-      <c r="H2132">
-        <v>55</v>
-      </c>
-      <c r="I2132">
-        <v>1</v>
-      </c>
-      <c r="J2132">
-        <v>11</v>
-      </c>
-      <c r="K2132">
-        <v>5</v>
-      </c>
-      <c r="L2132">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2133" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2133">
-        <v>2017</v>
-      </c>
-      <c r="B2133">
-        <v>3</v>
-      </c>
-      <c r="C2133" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2133" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2133">
-        <v>38</v>
-      </c>
-      <c r="F2133">
-        <v>114</v>
-      </c>
-      <c r="G2133">
-        <v>184</v>
-      </c>
-      <c r="H2133">
-        <v>552</v>
-      </c>
-      <c r="I2133">
-        <v>0</v>
-      </c>
-      <c r="J2133">
-        <v>0</v>
-      </c>
-      <c r="K2133">
-        <v>93</v>
-      </c>
-      <c r="L2133">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2134" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2134">
-        <v>2017</v>
-      </c>
-      <c r="B2134">
-        <v>3</v>
-      </c>
-      <c r="C2134" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2134" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2134">
-        <v>0</v>
-      </c>
-      <c r="F2134">
-        <v>0</v>
-      </c>
-      <c r="G2134">
-        <v>7</v>
-      </c>
-      <c r="H2134">
-        <v>77</v>
-      </c>
-      <c r="I2134">
-        <v>1</v>
-      </c>
-      <c r="J2134">
-        <v>11</v>
-      </c>
-      <c r="K2134">
-        <v>10</v>
-      </c>
-      <c r="L2134">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2135">
-        <v>2017</v>
-      </c>
-      <c r="B2135">
-        <v>3</v>
-      </c>
-      <c r="C2135" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2135" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2135">
-        <v>3081</v>
-      </c>
-      <c r="F2135">
-        <v>3081</v>
-      </c>
-      <c r="G2135">
-        <v>3128</v>
-      </c>
-      <c r="H2135">
-        <v>3128</v>
-      </c>
-      <c r="I2135">
-        <v>4420</v>
-      </c>
-      <c r="J2135">
-        <v>4420</v>
-      </c>
-      <c r="K2135">
-        <v>5015</v>
-      </c>
-      <c r="L2135">
-        <v>5015</v>
-      </c>
-    </row>
-    <row r="2136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2136">
-        <v>2017</v>
-      </c>
-      <c r="B2136">
-        <v>3</v>
-      </c>
-      <c r="C2136" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2136" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2136">
-        <v>3</v>
-      </c>
-      <c r="F2136">
-        <v>9</v>
-      </c>
-      <c r="G2136">
-        <v>4532</v>
-      </c>
-      <c r="H2136">
-        <v>13596</v>
-      </c>
-      <c r="I2136">
-        <v>-48</v>
-      </c>
-      <c r="J2136">
-        <v>-144</v>
-      </c>
-      <c r="K2136">
-        <v>4021</v>
-      </c>
-      <c r="L2136">
-        <v>12063</v>
-      </c>
-    </row>
-    <row r="2137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2137">
-        <v>2017</v>
-      </c>
-      <c r="B2137">
-        <v>3</v>
-      </c>
-      <c r="C2137" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2137" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2137">
-        <v>229</v>
-      </c>
-      <c r="F2137">
-        <v>3893</v>
-      </c>
-      <c r="G2137">
-        <v>441</v>
-      </c>
-      <c r="H2137">
-        <v>7497</v>
-      </c>
-      <c r="I2137">
-        <v>277</v>
-      </c>
-      <c r="J2137">
-        <v>4709</v>
-      </c>
-      <c r="K2137">
-        <v>350</v>
-      </c>
-      <c r="L2137">
-        <v>5950</v>
-      </c>
-    </row>
-    <row r="2138" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2138">
-        <v>2017</v>
-      </c>
-      <c r="B2138">
-        <v>3</v>
-      </c>
-      <c r="C2138" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2138" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2138">
-        <v>760</v>
-      </c>
-      <c r="F2138">
-        <v>760</v>
-      </c>
-      <c r="G2138">
-        <v>761</v>
-      </c>
-      <c r="H2138">
-        <v>761</v>
-      </c>
-      <c r="I2138">
-        <v>2714</v>
-      </c>
-      <c r="J2138">
-        <v>2714</v>
-      </c>
-      <c r="K2138">
-        <v>2714</v>
-      </c>
-      <c r="L2138">
-        <v>2714</v>
-      </c>
-    </row>
-    <row r="2139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2139">
-        <v>2017</v>
-      </c>
-      <c r="B2139">
-        <v>3</v>
-      </c>
-      <c r="C2139" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2139" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2139">
-        <v>12</v>
-      </c>
-      <c r="F2139">
-        <v>36</v>
-      </c>
-      <c r="G2139">
-        <v>2648</v>
-      </c>
-      <c r="H2139">
-        <v>7944</v>
-      </c>
-      <c r="I2139">
-        <v>9</v>
-      </c>
-      <c r="J2139">
-        <v>27</v>
-      </c>
-      <c r="K2139">
-        <v>2701</v>
-      </c>
-      <c r="L2139">
-        <v>8103</v>
-      </c>
-    </row>
-    <row r="2140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2140">
-        <v>2017</v>
-      </c>
-      <c r="B2140">
-        <v>3</v>
-      </c>
-      <c r="C2140" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2140" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2140">
-        <v>22</v>
-      </c>
-      <c r="F2140">
-        <v>374</v>
-      </c>
-      <c r="G2140">
-        <v>77</v>
-      </c>
-      <c r="H2140">
-        <v>1309</v>
-      </c>
-      <c r="I2140">
-        <v>39</v>
-      </c>
-      <c r="J2140">
-        <v>663</v>
-      </c>
-      <c r="K2140">
-        <v>102</v>
-      </c>
-      <c r="L2140">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="2141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2141">
-        <v>2017</v>
-      </c>
-      <c r="B2141">
-        <v>3</v>
-      </c>
-      <c r="C2141" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2141" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2141">
-        <v>0</v>
-      </c>
-      <c r="F2141">
-        <v>0</v>
-      </c>
-      <c r="G2141">
-        <v>0</v>
-      </c>
-      <c r="H2141">
-        <v>0</v>
-      </c>
-      <c r="I2141">
-        <v>727</v>
-      </c>
-      <c r="J2141">
-        <v>727</v>
-      </c>
-      <c r="K2141">
-        <v>1127</v>
-      </c>
-      <c r="L2141">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="2142" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2142">
-        <v>2017</v>
-      </c>
-      <c r="B2142">
-        <v>3</v>
-      </c>
-      <c r="C2142" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2142" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2142">
-        <v>0</v>
-      </c>
-      <c r="F2142">
-        <v>0</v>
-      </c>
-      <c r="G2142">
-        <v>1142</v>
-      </c>
-      <c r="H2142">
-        <v>3426</v>
-      </c>
-      <c r="I2142">
-        <v>-3</v>
-      </c>
-      <c r="J2142">
-        <v>-9</v>
-      </c>
-      <c r="K2142">
-        <v>922</v>
-      </c>
-      <c r="L2142">
-        <v>2766</v>
-      </c>
-    </row>
-    <row r="2143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2143">
-        <v>2017</v>
-      </c>
-      <c r="B2143">
-        <v>3</v>
-      </c>
-      <c r="C2143" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2143" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2143">
-        <v>0</v>
-      </c>
-      <c r="F2143">
-        <v>0</v>
-      </c>
-      <c r="G2143">
-        <v>40</v>
-      </c>
-      <c r="H2143">
-        <v>680</v>
-      </c>
-      <c r="I2143">
-        <v>165</v>
-      </c>
-      <c r="J2143">
-        <v>2805</v>
-      </c>
-      <c r="K2143">
-        <v>223</v>
-      </c>
-      <c r="L2143">
-        <v>3791</v>
-      </c>
-    </row>
-    <row r="2144" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2144">
-        <v>2017</v>
-      </c>
-      <c r="B2144">
-        <v>3</v>
-      </c>
-      <c r="C2144" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2144" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2144">
-        <v>1</v>
-      </c>
-      <c r="F2144">
-        <v>11</v>
-      </c>
-      <c r="G2144">
-        <v>3</v>
-      </c>
-      <c r="H2144">
-        <v>33</v>
-      </c>
-      <c r="I2144">
-        <v>3</v>
-      </c>
-      <c r="J2144">
-        <v>33</v>
-      </c>
-      <c r="K2144">
-        <v>8</v>
-      </c>
-      <c r="L2144">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2145">
-        <v>2017</v>
-      </c>
-      <c r="B2145">
-        <v>3</v>
-      </c>
-      <c r="C2145" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2145" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2145">
-        <v>172</v>
-      </c>
-      <c r="F2145">
-        <v>172</v>
-      </c>
-      <c r="G2145">
-        <v>405</v>
-      </c>
-      <c r="H2145">
-        <v>405</v>
-      </c>
-      <c r="I2145">
-        <v>1914</v>
-      </c>
-      <c r="J2145">
-        <v>1914</v>
-      </c>
-      <c r="K2145">
-        <v>3142</v>
-      </c>
-      <c r="L2145">
-        <v>3142</v>
-      </c>
-    </row>
-    <row r="2146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2146">
-        <v>2017</v>
-      </c>
-      <c r="B2146">
-        <v>3</v>
-      </c>
-      <c r="C2146" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2146" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2146">
-        <v>198</v>
-      </c>
-      <c r="F2146">
-        <v>594</v>
-      </c>
-      <c r="G2146">
-        <v>2126</v>
-      </c>
-      <c r="H2146">
-        <v>6378</v>
-      </c>
-      <c r="I2146">
-        <v>12</v>
-      </c>
-      <c r="J2146">
-        <v>36</v>
-      </c>
-      <c r="K2146">
-        <v>1889</v>
-      </c>
-      <c r="L2146">
-        <v>5667</v>
-      </c>
-    </row>
-    <row r="2147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2147">
-        <v>2017</v>
-      </c>
-      <c r="B2147">
-        <v>3</v>
-      </c>
-      <c r="C2147" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2147" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2147">
-        <v>24</v>
-      </c>
-      <c r="F2147">
-        <v>408</v>
-      </c>
-      <c r="G2147">
-        <v>25</v>
-      </c>
-      <c r="H2147">
-        <v>425</v>
-      </c>
-      <c r="I2147">
-        <v>42</v>
-      </c>
-      <c r="J2147">
-        <v>714</v>
-      </c>
-      <c r="K2147">
-        <v>44</v>
-      </c>
-      <c r="L2147">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="2148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2148">
-        <v>2017</v>
-      </c>
-      <c r="B2148">
-        <v>3</v>
-      </c>
-      <c r="C2148" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2148" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2148">
-        <v>0</v>
-      </c>
-      <c r="F2148">
-        <v>0</v>
-      </c>
-      <c r="G2148">
-        <v>20</v>
-      </c>
-      <c r="H2148">
-        <v>226</v>
-      </c>
-      <c r="I2148">
-        <v>8</v>
-      </c>
-      <c r="J2148">
-        <v>89</v>
-      </c>
-      <c r="K2148">
-        <v>20</v>
-      </c>
-      <c r="L2148">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2149">
-        <v>2017</v>
-      </c>
-      <c r="B2149">
-        <v>3</v>
-      </c>
-      <c r="C2149" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2149" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2149">
-        <v>140</v>
-      </c>
-      <c r="F2149">
-        <v>140</v>
-      </c>
-      <c r="G2149">
-        <v>140</v>
-      </c>
-      <c r="H2149">
-        <v>140</v>
-      </c>
-      <c r="I2149">
-        <v>0</v>
-      </c>
-      <c r="J2149">
-        <v>0</v>
-      </c>
-      <c r="K2149">
-        <v>0</v>
-      </c>
-      <c r="L2149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2150">
-        <v>2017</v>
-      </c>
-      <c r="B2150">
-        <v>3</v>
-      </c>
-      <c r="C2150" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2150" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2150">
-        <v>0</v>
-      </c>
-      <c r="F2150">
-        <v>0</v>
-      </c>
-      <c r="G2150">
-        <v>4</v>
-      </c>
-      <c r="H2150">
-        <v>12</v>
-      </c>
-      <c r="I2150">
-        <v>0</v>
-      </c>
-      <c r="J2150">
-        <v>0</v>
-      </c>
-      <c r="K2150">
-        <v>1</v>
-      </c>
-      <c r="L2150">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2151" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2151">
-        <v>2017</v>
-      </c>
-      <c r="B2151">
-        <v>3</v>
-      </c>
-      <c r="C2151" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2151" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2151">
-        <v>2</v>
-      </c>
-      <c r="F2151">
-        <v>22</v>
-      </c>
-      <c r="G2151">
-        <v>4</v>
-      </c>
-      <c r="H2151">
-        <v>44</v>
-      </c>
-      <c r="I2151">
-        <v>2</v>
-      </c>
-      <c r="J2151">
-        <v>22</v>
-      </c>
-      <c r="K2151">
-        <v>2</v>
-      </c>
-      <c r="L2151">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2152">
-        <v>2017</v>
-      </c>
-      <c r="B2152">
-        <v>3</v>
-      </c>
-      <c r="C2152" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2152" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2152">
-        <v>28</v>
-      </c>
-      <c r="F2152">
-        <v>28</v>
-      </c>
-      <c r="G2152">
-        <v>28</v>
-      </c>
-      <c r="H2152">
-        <v>28</v>
-      </c>
-      <c r="I2152">
-        <v>30</v>
-      </c>
-      <c r="J2152">
-        <v>30</v>
-      </c>
-      <c r="K2152">
-        <v>30</v>
-      </c>
-      <c r="L2152">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2153">
-        <v>2017</v>
-      </c>
-      <c r="B2153">
-        <v>3</v>
-      </c>
-      <c r="C2153" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2153" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2153">
-        <v>24</v>
-      </c>
-      <c r="F2153">
-        <v>72</v>
-      </c>
-      <c r="G2153">
-        <v>214</v>
-      </c>
-      <c r="H2153">
-        <v>642</v>
-      </c>
-      <c r="I2153">
-        <v>-2</v>
-      </c>
-      <c r="J2153">
-        <v>-6</v>
-      </c>
-      <c r="K2153">
-        <v>275</v>
-      </c>
-      <c r="L2153">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="2154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2154">
-        <v>2017</v>
-      </c>
-      <c r="B2154">
-        <v>3</v>
-      </c>
-      <c r="C2154" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2154" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2154">
-        <v>0</v>
-      </c>
-      <c r="F2154">
-        <v>0</v>
-      </c>
-      <c r="G2154">
-        <v>0</v>
-      </c>
-      <c r="H2154">
-        <v>0</v>
-      </c>
-      <c r="I2154">
-        <v>3</v>
-      </c>
-      <c r="J2154">
-        <v>51</v>
-      </c>
-      <c r="K2154">
-        <v>3</v>
-      </c>
-      <c r="L2154">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2155" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2155">
-        <v>2017</v>
-      </c>
-      <c r="B2155">
-        <v>3</v>
-      </c>
-      <c r="C2155" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2155" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2155">
-        <v>1</v>
-      </c>
-      <c r="F2155">
-        <v>11</v>
-      </c>
-      <c r="G2155">
-        <v>2</v>
-      </c>
-      <c r="H2155">
-        <v>22</v>
-      </c>
-      <c r="I2155">
-        <v>0</v>
-      </c>
-      <c r="J2155">
-        <v>0</v>
-      </c>
-      <c r="K2155">
-        <v>3</v>
-      </c>
-      <c r="L2155">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2156" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2156">
-        <v>2017</v>
-      </c>
-      <c r="B2156">
-        <v>3</v>
-      </c>
-      <c r="C2156" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2156" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2156">
-        <v>0</v>
-      </c>
-      <c r="F2156">
-        <v>0</v>
-      </c>
-      <c r="G2156">
-        <v>499</v>
-      </c>
-      <c r="H2156">
-        <v>1497</v>
-      </c>
-      <c r="I2156">
-        <v>0</v>
-      </c>
-      <c r="J2156">
-        <v>0</v>
-      </c>
-      <c r="K2156">
-        <v>208</v>
-      </c>
-      <c r="L2156">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="2157" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2157">
-        <v>2017</v>
-      </c>
-      <c r="B2157">
-        <v>3</v>
-      </c>
-      <c r="C2157" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2157" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2157">
-        <v>4</v>
-      </c>
-      <c r="F2157">
-        <v>68</v>
-      </c>
-      <c r="G2157">
-        <v>5</v>
-      </c>
-      <c r="H2157">
-        <v>85</v>
-      </c>
-      <c r="I2157">
-        <v>0</v>
-      </c>
-      <c r="J2157">
-        <v>0</v>
-      </c>
-      <c r="K2157">
-        <v>0</v>
-      </c>
-      <c r="L2157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2158" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2158">
-        <v>2017</v>
-      </c>
-      <c r="B2158">
-        <v>3</v>
-      </c>
-      <c r="C2158" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2158" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2158">
-        <v>1</v>
-      </c>
-      <c r="F2158">
-        <v>11</v>
-      </c>
-      <c r="G2158">
-        <v>6</v>
-      </c>
-      <c r="H2158">
-        <v>66</v>
-      </c>
-      <c r="I2158">
-        <v>0</v>
-      </c>
-      <c r="J2158">
-        <v>0</v>
-      </c>
-      <c r="K2158">
-        <v>4</v>
-      </c>
-      <c r="L2158">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2159" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2159">
-        <v>2017</v>
-      </c>
-      <c r="B2159">
-        <v>3</v>
-      </c>
-      <c r="C2159" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2159" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2159">
-        <v>1730</v>
-      </c>
-      <c r="F2159">
-        <v>1730</v>
-      </c>
-      <c r="G2159">
-        <v>2164</v>
-      </c>
-      <c r="H2159">
-        <v>2164</v>
-      </c>
-      <c r="I2159">
-        <v>1790</v>
-      </c>
-      <c r="J2159">
-        <v>1790</v>
-      </c>
-      <c r="K2159">
-        <v>2335</v>
-      </c>
-      <c r="L2159">
-        <v>2335</v>
-      </c>
-    </row>
-    <row r="2160" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2160">
-        <v>2017</v>
-      </c>
-      <c r="B2160">
-        <v>3</v>
-      </c>
-      <c r="C2160" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2160" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2160">
-        <v>10</v>
-      </c>
-      <c r="F2160">
-        <v>30</v>
-      </c>
-      <c r="G2160">
-        <v>3294</v>
-      </c>
-      <c r="H2160">
-        <v>9882</v>
-      </c>
-      <c r="I2160">
-        <v>-19</v>
-      </c>
-      <c r="J2160">
-        <v>-57</v>
-      </c>
-      <c r="K2160">
-        <v>2339</v>
-      </c>
-      <c r="L2160">
-        <v>7017</v>
-      </c>
-    </row>
-    <row r="2161" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2161">
-        <v>2017</v>
-      </c>
-      <c r="B2161">
-        <v>3</v>
-      </c>
-      <c r="C2161" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2161" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2161">
-        <v>99</v>
-      </c>
-      <c r="F2161">
-        <v>1683</v>
-      </c>
-      <c r="G2161">
-        <v>108</v>
-      </c>
-      <c r="H2161">
-        <v>1836</v>
-      </c>
-      <c r="I2161">
-        <v>76</v>
-      </c>
-      <c r="J2161">
-        <v>1292</v>
-      </c>
-      <c r="K2161">
-        <v>105</v>
-      </c>
-      <c r="L2161">
-        <v>1785</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix for filter and updated Seeded Acres report
</commit_message>
<xml_diff>
--- a/UploadedFiles/SeededAcres.xlsx
+++ b/UploadedFiles/SeededAcres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4250" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="43">
   <si>
     <t>FiscalYear</t>
   </si>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2120" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2169" totalsRowShown="0">
   <tableColumns count="12">
     <tableColumn id="1" name="FiscalYear"/>
     <tableColumn id="2" name="FiscalPeriod"/>
@@ -495,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2120"/>
+  <dimension ref="A1:L2169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -81074,6 +81074,1868 @@
         <v>108</v>
       </c>
     </row>
+    <row r="2121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2121">
+        <v>2017</v>
+      </c>
+      <c r="B2121">
+        <v>3</v>
+      </c>
+      <c r="C2121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2121">
+        <v>4</v>
+      </c>
+      <c r="F2121">
+        <v>44</v>
+      </c>
+      <c r="G2121">
+        <v>4</v>
+      </c>
+      <c r="H2121">
+        <v>44</v>
+      </c>
+      <c r="I2121">
+        <v>0</v>
+      </c>
+      <c r="J2121">
+        <v>0</v>
+      </c>
+      <c r="K2121">
+        <v>0</v>
+      </c>
+      <c r="L2121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2122">
+        <v>2017</v>
+      </c>
+      <c r="B2122">
+        <v>3</v>
+      </c>
+      <c r="C2122" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2122" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2122">
+        <v>2278</v>
+      </c>
+      <c r="F2122">
+        <v>2278</v>
+      </c>
+      <c r="G2122">
+        <v>2278</v>
+      </c>
+      <c r="H2122">
+        <v>2278</v>
+      </c>
+      <c r="I2122">
+        <v>958</v>
+      </c>
+      <c r="J2122">
+        <v>958</v>
+      </c>
+      <c r="K2122">
+        <v>1045</v>
+      </c>
+      <c r="L2122">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2123">
+        <v>2017</v>
+      </c>
+      <c r="B2123">
+        <v>3</v>
+      </c>
+      <c r="C2123" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2123" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2123">
+        <v>12</v>
+      </c>
+      <c r="F2123">
+        <v>36</v>
+      </c>
+      <c r="G2123">
+        <v>809</v>
+      </c>
+      <c r="H2123">
+        <v>2427</v>
+      </c>
+      <c r="I2123">
+        <v>7</v>
+      </c>
+      <c r="J2123">
+        <v>21</v>
+      </c>
+      <c r="K2123">
+        <v>536</v>
+      </c>
+      <c r="L2123">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2124">
+        <v>2017</v>
+      </c>
+      <c r="B2124">
+        <v>3</v>
+      </c>
+      <c r="C2124" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2124" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2124">
+        <v>36</v>
+      </c>
+      <c r="F2124">
+        <v>612</v>
+      </c>
+      <c r="G2124">
+        <v>38</v>
+      </c>
+      <c r="H2124">
+        <v>646</v>
+      </c>
+      <c r="I2124">
+        <v>1</v>
+      </c>
+      <c r="J2124">
+        <v>17</v>
+      </c>
+      <c r="K2124">
+        <v>37</v>
+      </c>
+      <c r="L2124">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2125">
+        <v>2017</v>
+      </c>
+      <c r="B2125">
+        <v>3</v>
+      </c>
+      <c r="C2125" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2125" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2125">
+        <v>7</v>
+      </c>
+      <c r="F2125">
+        <v>77</v>
+      </c>
+      <c r="G2125">
+        <v>22</v>
+      </c>
+      <c r="H2125">
+        <v>242</v>
+      </c>
+      <c r="I2125">
+        <v>12</v>
+      </c>
+      <c r="J2125">
+        <v>132</v>
+      </c>
+      <c r="K2125">
+        <v>38</v>
+      </c>
+      <c r="L2125">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2126">
+        <v>2017</v>
+      </c>
+      <c r="B2126">
+        <v>3</v>
+      </c>
+      <c r="C2126" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2126" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2126">
+        <v>12</v>
+      </c>
+      <c r="F2126">
+        <v>36</v>
+      </c>
+      <c r="G2126">
+        <v>13</v>
+      </c>
+      <c r="H2126">
+        <v>39</v>
+      </c>
+      <c r="I2126">
+        <v>23</v>
+      </c>
+      <c r="J2126">
+        <v>69</v>
+      </c>
+      <c r="K2126">
+        <v>77</v>
+      </c>
+      <c r="L2126">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2127">
+        <v>2017</v>
+      </c>
+      <c r="B2127">
+        <v>3</v>
+      </c>
+      <c r="C2127" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2127" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2127">
+        <v>0</v>
+      </c>
+      <c r="F2127">
+        <v>0</v>
+      </c>
+      <c r="G2127">
+        <v>3</v>
+      </c>
+      <c r="H2127">
+        <v>33</v>
+      </c>
+      <c r="I2127">
+        <v>1</v>
+      </c>
+      <c r="J2127">
+        <v>11</v>
+      </c>
+      <c r="K2127">
+        <v>2</v>
+      </c>
+      <c r="L2127">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2128">
+        <v>2017</v>
+      </c>
+      <c r="B2128">
+        <v>3</v>
+      </c>
+      <c r="C2128" s="1">
+        <v>140</v>
+      </c>
+      <c r="D2128" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2128">
+        <v>39</v>
+      </c>
+      <c r="F2128">
+        <v>663</v>
+      </c>
+      <c r="G2128">
+        <v>39</v>
+      </c>
+      <c r="H2128">
+        <v>663</v>
+      </c>
+      <c r="I2128">
+        <v>0</v>
+      </c>
+      <c r="J2128">
+        <v>0</v>
+      </c>
+      <c r="K2128">
+        <v>0</v>
+      </c>
+      <c r="L2128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2129">
+        <v>2017</v>
+      </c>
+      <c r="B2129">
+        <v>3</v>
+      </c>
+      <c r="C2129" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2129" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2129">
+        <v>2760</v>
+      </c>
+      <c r="F2129">
+        <v>2760</v>
+      </c>
+      <c r="G2129">
+        <v>2760</v>
+      </c>
+      <c r="H2129">
+        <v>2760</v>
+      </c>
+      <c r="I2129">
+        <v>0</v>
+      </c>
+      <c r="J2129">
+        <v>0</v>
+      </c>
+      <c r="K2129">
+        <v>0</v>
+      </c>
+      <c r="L2129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2130">
+        <v>2017</v>
+      </c>
+      <c r="B2130">
+        <v>3</v>
+      </c>
+      <c r="C2130" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2130" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2130">
+        <v>0</v>
+      </c>
+      <c r="F2130">
+        <v>0</v>
+      </c>
+      <c r="G2130">
+        <v>227</v>
+      </c>
+      <c r="H2130">
+        <v>681</v>
+      </c>
+      <c r="I2130">
+        <v>72</v>
+      </c>
+      <c r="J2130">
+        <v>216</v>
+      </c>
+      <c r="K2130">
+        <v>200</v>
+      </c>
+      <c r="L2130">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2131">
+        <v>2017</v>
+      </c>
+      <c r="B2131">
+        <v>3</v>
+      </c>
+      <c r="C2131" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2131" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2131">
+        <v>0</v>
+      </c>
+      <c r="F2131">
+        <v>0</v>
+      </c>
+      <c r="G2131">
+        <v>0</v>
+      </c>
+      <c r="H2131">
+        <v>0</v>
+      </c>
+      <c r="I2131">
+        <v>-1</v>
+      </c>
+      <c r="J2131">
+        <v>-17</v>
+      </c>
+      <c r="K2131">
+        <v>3</v>
+      </c>
+      <c r="L2131">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2132">
+        <v>2017</v>
+      </c>
+      <c r="B2132">
+        <v>3</v>
+      </c>
+      <c r="C2132" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2132" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2132">
+        <v>1</v>
+      </c>
+      <c r="F2132">
+        <v>11</v>
+      </c>
+      <c r="G2132">
+        <v>2</v>
+      </c>
+      <c r="H2132">
+        <v>22</v>
+      </c>
+      <c r="I2132">
+        <v>0</v>
+      </c>
+      <c r="J2132">
+        <v>0</v>
+      </c>
+      <c r="K2132">
+        <v>2</v>
+      </c>
+      <c r="L2132">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2133">
+        <v>2017</v>
+      </c>
+      <c r="B2133">
+        <v>3</v>
+      </c>
+      <c r="C2133" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2133" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2133">
+        <v>0</v>
+      </c>
+      <c r="F2133">
+        <v>0</v>
+      </c>
+      <c r="G2133">
+        <v>69</v>
+      </c>
+      <c r="H2133">
+        <v>207</v>
+      </c>
+      <c r="I2133">
+        <v>0</v>
+      </c>
+      <c r="J2133">
+        <v>0</v>
+      </c>
+      <c r="K2133">
+        <v>94</v>
+      </c>
+      <c r="L2133">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2134">
+        <v>2017</v>
+      </c>
+      <c r="B2134">
+        <v>3</v>
+      </c>
+      <c r="C2134" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2134" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2134">
+        <v>0</v>
+      </c>
+      <c r="F2134">
+        <v>0</v>
+      </c>
+      <c r="G2134">
+        <v>6</v>
+      </c>
+      <c r="H2134">
+        <v>102</v>
+      </c>
+      <c r="I2134">
+        <v>0</v>
+      </c>
+      <c r="J2134">
+        <v>0</v>
+      </c>
+      <c r="K2134">
+        <v>0</v>
+      </c>
+      <c r="L2134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2135">
+        <v>2017</v>
+      </c>
+      <c r="B2135">
+        <v>3</v>
+      </c>
+      <c r="C2135" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2135" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2135">
+        <v>1</v>
+      </c>
+      <c r="F2135">
+        <v>11</v>
+      </c>
+      <c r="G2135">
+        <v>5</v>
+      </c>
+      <c r="H2135">
+        <v>55</v>
+      </c>
+      <c r="I2135">
+        <v>1</v>
+      </c>
+      <c r="J2135">
+        <v>11</v>
+      </c>
+      <c r="K2135">
+        <v>5</v>
+      </c>
+      <c r="L2135">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2136">
+        <v>2017</v>
+      </c>
+      <c r="B2136">
+        <v>3</v>
+      </c>
+      <c r="C2136" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2136" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2136">
+        <v>38</v>
+      </c>
+      <c r="F2136">
+        <v>114</v>
+      </c>
+      <c r="G2136">
+        <v>184</v>
+      </c>
+      <c r="H2136">
+        <v>552</v>
+      </c>
+      <c r="I2136">
+        <v>0</v>
+      </c>
+      <c r="J2136">
+        <v>0</v>
+      </c>
+      <c r="K2136">
+        <v>93</v>
+      </c>
+      <c r="L2136">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2137">
+        <v>2017</v>
+      </c>
+      <c r="B2137">
+        <v>3</v>
+      </c>
+      <c r="C2137" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2137" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2137">
+        <v>0</v>
+      </c>
+      <c r="F2137">
+        <v>0</v>
+      </c>
+      <c r="G2137">
+        <v>7</v>
+      </c>
+      <c r="H2137">
+        <v>77</v>
+      </c>
+      <c r="I2137">
+        <v>1</v>
+      </c>
+      <c r="J2137">
+        <v>11</v>
+      </c>
+      <c r="K2137">
+        <v>10</v>
+      </c>
+      <c r="L2137">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2138">
+        <v>2017</v>
+      </c>
+      <c r="B2138">
+        <v>3</v>
+      </c>
+      <c r="C2138" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2138" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2138">
+        <v>6861</v>
+      </c>
+      <c r="F2138">
+        <v>6861</v>
+      </c>
+      <c r="G2138">
+        <v>6908</v>
+      </c>
+      <c r="H2138">
+        <v>6908</v>
+      </c>
+      <c r="I2138">
+        <v>4420</v>
+      </c>
+      <c r="J2138">
+        <v>4420</v>
+      </c>
+      <c r="K2138">
+        <v>5015</v>
+      </c>
+      <c r="L2138">
+        <v>5015</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2139">
+        <v>2017</v>
+      </c>
+      <c r="B2139">
+        <v>3</v>
+      </c>
+      <c r="C2139" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2139" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2139">
+        <v>-98</v>
+      </c>
+      <c r="F2139">
+        <v>-294</v>
+      </c>
+      <c r="G2139">
+        <v>4431</v>
+      </c>
+      <c r="H2139">
+        <v>13293</v>
+      </c>
+      <c r="I2139">
+        <v>-48</v>
+      </c>
+      <c r="J2139">
+        <v>-144</v>
+      </c>
+      <c r="K2139">
+        <v>4021</v>
+      </c>
+      <c r="L2139">
+        <v>12063</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2140">
+        <v>2017</v>
+      </c>
+      <c r="B2140">
+        <v>3</v>
+      </c>
+      <c r="C2140" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2140" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2140">
+        <v>431</v>
+      </c>
+      <c r="F2140">
+        <v>7327</v>
+      </c>
+      <c r="G2140">
+        <v>643</v>
+      </c>
+      <c r="H2140">
+        <v>10931</v>
+      </c>
+      <c r="I2140">
+        <v>277</v>
+      </c>
+      <c r="J2140">
+        <v>4709</v>
+      </c>
+      <c r="K2140">
+        <v>350</v>
+      </c>
+      <c r="L2140">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="2141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2141">
+        <v>2017</v>
+      </c>
+      <c r="B2141">
+        <v>3</v>
+      </c>
+      <c r="C2141" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2141" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2141">
+        <v>1282</v>
+      </c>
+      <c r="F2141">
+        <v>1282</v>
+      </c>
+      <c r="G2141">
+        <v>1283</v>
+      </c>
+      <c r="H2141">
+        <v>1283</v>
+      </c>
+      <c r="I2141">
+        <v>2714</v>
+      </c>
+      <c r="J2141">
+        <v>2714</v>
+      </c>
+      <c r="K2141">
+        <v>2714</v>
+      </c>
+      <c r="L2141">
+        <v>2714</v>
+      </c>
+    </row>
+    <row r="2142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2142">
+        <v>2017</v>
+      </c>
+      <c r="B2142">
+        <v>3</v>
+      </c>
+      <c r="C2142" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2142" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2142">
+        <v>104</v>
+      </c>
+      <c r="F2142">
+        <v>312</v>
+      </c>
+      <c r="G2142">
+        <v>2740</v>
+      </c>
+      <c r="H2142">
+        <v>8220</v>
+      </c>
+      <c r="I2142">
+        <v>9</v>
+      </c>
+      <c r="J2142">
+        <v>27</v>
+      </c>
+      <c r="K2142">
+        <v>2701</v>
+      </c>
+      <c r="L2142">
+        <v>8103</v>
+      </c>
+    </row>
+    <row r="2143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2143">
+        <v>2017</v>
+      </c>
+      <c r="B2143">
+        <v>3</v>
+      </c>
+      <c r="C2143" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2143" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2143">
+        <v>74</v>
+      </c>
+      <c r="F2143">
+        <v>1258</v>
+      </c>
+      <c r="G2143">
+        <v>129</v>
+      </c>
+      <c r="H2143">
+        <v>2193</v>
+      </c>
+      <c r="I2143">
+        <v>39</v>
+      </c>
+      <c r="J2143">
+        <v>663</v>
+      </c>
+      <c r="K2143">
+        <v>102</v>
+      </c>
+      <c r="L2143">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="2144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2144">
+        <v>2017</v>
+      </c>
+      <c r="B2144">
+        <v>3</v>
+      </c>
+      <c r="C2144" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2144" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2144">
+        <v>3431</v>
+      </c>
+      <c r="F2144">
+        <v>3431</v>
+      </c>
+      <c r="G2144">
+        <v>3431</v>
+      </c>
+      <c r="H2144">
+        <v>3431</v>
+      </c>
+      <c r="I2144">
+        <v>727</v>
+      </c>
+      <c r="J2144">
+        <v>727</v>
+      </c>
+      <c r="K2144">
+        <v>1127</v>
+      </c>
+      <c r="L2144">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="2145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2145">
+        <v>2017</v>
+      </c>
+      <c r="B2145">
+        <v>3</v>
+      </c>
+      <c r="C2145" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2145" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2145">
+        <v>14</v>
+      </c>
+      <c r="F2145">
+        <v>42</v>
+      </c>
+      <c r="G2145">
+        <v>1156</v>
+      </c>
+      <c r="H2145">
+        <v>3468</v>
+      </c>
+      <c r="I2145">
+        <v>-3</v>
+      </c>
+      <c r="J2145">
+        <v>-9</v>
+      </c>
+      <c r="K2145">
+        <v>922</v>
+      </c>
+      <c r="L2145">
+        <v>2766</v>
+      </c>
+    </row>
+    <row r="2146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2146">
+        <v>2017</v>
+      </c>
+      <c r="B2146">
+        <v>3</v>
+      </c>
+      <c r="C2146" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2146" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2146">
+        <v>235</v>
+      </c>
+      <c r="F2146">
+        <v>3995</v>
+      </c>
+      <c r="G2146">
+        <v>275</v>
+      </c>
+      <c r="H2146">
+        <v>4675</v>
+      </c>
+      <c r="I2146">
+        <v>165</v>
+      </c>
+      <c r="J2146">
+        <v>2805</v>
+      </c>
+      <c r="K2146">
+        <v>223</v>
+      </c>
+      <c r="L2146">
+        <v>3791</v>
+      </c>
+    </row>
+    <row r="2147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2147">
+        <v>2017</v>
+      </c>
+      <c r="B2147">
+        <v>3</v>
+      </c>
+      <c r="C2147" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2147" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2147">
+        <v>2</v>
+      </c>
+      <c r="F2147">
+        <v>22</v>
+      </c>
+      <c r="G2147">
+        <v>4</v>
+      </c>
+      <c r="H2147">
+        <v>44</v>
+      </c>
+      <c r="I2147">
+        <v>3</v>
+      </c>
+      <c r="J2147">
+        <v>33</v>
+      </c>
+      <c r="K2147">
+        <v>8</v>
+      </c>
+      <c r="L2147">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2148">
+        <v>2017</v>
+      </c>
+      <c r="B2148">
+        <v>3</v>
+      </c>
+      <c r="C2148" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2148" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2148">
+        <v>5634</v>
+      </c>
+      <c r="F2148">
+        <v>5634</v>
+      </c>
+      <c r="G2148">
+        <v>5868</v>
+      </c>
+      <c r="H2148">
+        <v>5868</v>
+      </c>
+      <c r="I2148">
+        <v>1914</v>
+      </c>
+      <c r="J2148">
+        <v>1914</v>
+      </c>
+      <c r="K2148">
+        <v>3142</v>
+      </c>
+      <c r="L2148">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="2149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2149">
+        <v>2017</v>
+      </c>
+      <c r="B2149">
+        <v>3</v>
+      </c>
+      <c r="C2149" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2149" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2149">
+        <v>227</v>
+      </c>
+      <c r="F2149">
+        <v>681</v>
+      </c>
+      <c r="G2149">
+        <v>2155</v>
+      </c>
+      <c r="H2149">
+        <v>6465</v>
+      </c>
+      <c r="I2149">
+        <v>12</v>
+      </c>
+      <c r="J2149">
+        <v>36</v>
+      </c>
+      <c r="K2149">
+        <v>1889</v>
+      </c>
+      <c r="L2149">
+        <v>5667</v>
+      </c>
+    </row>
+    <row r="2150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2150">
+        <v>2017</v>
+      </c>
+      <c r="B2150">
+        <v>3</v>
+      </c>
+      <c r="C2150" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2150" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2150">
+        <v>43</v>
+      </c>
+      <c r="F2150">
+        <v>731</v>
+      </c>
+      <c r="G2150">
+        <v>44</v>
+      </c>
+      <c r="H2150">
+        <v>748</v>
+      </c>
+      <c r="I2150">
+        <v>42</v>
+      </c>
+      <c r="J2150">
+        <v>714</v>
+      </c>
+      <c r="K2150">
+        <v>44</v>
+      </c>
+      <c r="L2150">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2151">
+        <v>2017</v>
+      </c>
+      <c r="B2151">
+        <v>3</v>
+      </c>
+      <c r="C2151" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2151" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2151">
+        <v>3</v>
+      </c>
+      <c r="F2151">
+        <v>36</v>
+      </c>
+      <c r="G2151">
+        <v>23</v>
+      </c>
+      <c r="H2151">
+        <v>262</v>
+      </c>
+      <c r="I2151">
+        <v>8</v>
+      </c>
+      <c r="J2151">
+        <v>89</v>
+      </c>
+      <c r="K2151">
+        <v>20</v>
+      </c>
+      <c r="L2151">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2152">
+        <v>2017</v>
+      </c>
+      <c r="B2152">
+        <v>3</v>
+      </c>
+      <c r="C2152" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2152" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2152">
+        <v>140</v>
+      </c>
+      <c r="F2152">
+        <v>140</v>
+      </c>
+      <c r="G2152">
+        <v>140</v>
+      </c>
+      <c r="H2152">
+        <v>140</v>
+      </c>
+      <c r="I2152">
+        <v>0</v>
+      </c>
+      <c r="J2152">
+        <v>0</v>
+      </c>
+      <c r="K2152">
+        <v>0</v>
+      </c>
+      <c r="L2152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2153">
+        <v>2017</v>
+      </c>
+      <c r="B2153">
+        <v>3</v>
+      </c>
+      <c r="C2153" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2153" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2153">
+        <v>0</v>
+      </c>
+      <c r="F2153">
+        <v>0</v>
+      </c>
+      <c r="G2153">
+        <v>4</v>
+      </c>
+      <c r="H2153">
+        <v>12</v>
+      </c>
+      <c r="I2153">
+        <v>0</v>
+      </c>
+      <c r="J2153">
+        <v>0</v>
+      </c>
+      <c r="K2153">
+        <v>1</v>
+      </c>
+      <c r="L2153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2154">
+        <v>2017</v>
+      </c>
+      <c r="B2154">
+        <v>3</v>
+      </c>
+      <c r="C2154" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2154" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2154">
+        <v>-1</v>
+      </c>
+      <c r="F2154">
+        <v>-17</v>
+      </c>
+      <c r="G2154">
+        <v>-1</v>
+      </c>
+      <c r="H2154">
+        <v>-17</v>
+      </c>
+      <c r="I2154">
+        <v>0</v>
+      </c>
+      <c r="J2154">
+        <v>0</v>
+      </c>
+      <c r="K2154">
+        <v>0</v>
+      </c>
+      <c r="L2154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2155">
+        <v>2017</v>
+      </c>
+      <c r="B2155">
+        <v>3</v>
+      </c>
+      <c r="C2155" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2155" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2155">
+        <v>3</v>
+      </c>
+      <c r="F2155">
+        <v>33</v>
+      </c>
+      <c r="G2155">
+        <v>5</v>
+      </c>
+      <c r="H2155">
+        <v>55</v>
+      </c>
+      <c r="I2155">
+        <v>2</v>
+      </c>
+      <c r="J2155">
+        <v>22</v>
+      </c>
+      <c r="K2155">
+        <v>2</v>
+      </c>
+      <c r="L2155">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2156">
+        <v>2017</v>
+      </c>
+      <c r="B2156">
+        <v>3</v>
+      </c>
+      <c r="C2156" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2156" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2156">
+        <v>63</v>
+      </c>
+      <c r="F2156">
+        <v>63</v>
+      </c>
+      <c r="G2156">
+        <v>63</v>
+      </c>
+      <c r="H2156">
+        <v>63</v>
+      </c>
+      <c r="I2156">
+        <v>30</v>
+      </c>
+      <c r="J2156">
+        <v>30</v>
+      </c>
+      <c r="K2156">
+        <v>30</v>
+      </c>
+      <c r="L2156">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2157">
+        <v>2017</v>
+      </c>
+      <c r="B2157">
+        <v>3</v>
+      </c>
+      <c r="C2157" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2157" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2157">
+        <v>22</v>
+      </c>
+      <c r="F2157">
+        <v>66</v>
+      </c>
+      <c r="G2157">
+        <v>212</v>
+      </c>
+      <c r="H2157">
+        <v>636</v>
+      </c>
+      <c r="I2157">
+        <v>-2</v>
+      </c>
+      <c r="J2157">
+        <v>-6</v>
+      </c>
+      <c r="K2157">
+        <v>275</v>
+      </c>
+      <c r="L2157">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2158">
+        <v>2017</v>
+      </c>
+      <c r="B2158">
+        <v>3</v>
+      </c>
+      <c r="C2158" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2158" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2158">
+        <v>0</v>
+      </c>
+      <c r="F2158">
+        <v>0</v>
+      </c>
+      <c r="G2158">
+        <v>0</v>
+      </c>
+      <c r="H2158">
+        <v>0</v>
+      </c>
+      <c r="I2158">
+        <v>3</v>
+      </c>
+      <c r="J2158">
+        <v>51</v>
+      </c>
+      <c r="K2158">
+        <v>3</v>
+      </c>
+      <c r="L2158">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2159">
+        <v>2017</v>
+      </c>
+      <c r="B2159">
+        <v>3</v>
+      </c>
+      <c r="C2159" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2159" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2159">
+        <v>1</v>
+      </c>
+      <c r="F2159">
+        <v>11</v>
+      </c>
+      <c r="G2159">
+        <v>2</v>
+      </c>
+      <c r="H2159">
+        <v>22</v>
+      </c>
+      <c r="I2159">
+        <v>0</v>
+      </c>
+      <c r="J2159">
+        <v>0</v>
+      </c>
+      <c r="K2159">
+        <v>3</v>
+      </c>
+      <c r="L2159">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2160">
+        <v>2017</v>
+      </c>
+      <c r="B2160">
+        <v>3</v>
+      </c>
+      <c r="C2160" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2160" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2160">
+        <v>0</v>
+      </c>
+      <c r="F2160">
+        <v>0</v>
+      </c>
+      <c r="G2160">
+        <v>499</v>
+      </c>
+      <c r="H2160">
+        <v>1497</v>
+      </c>
+      <c r="I2160">
+        <v>0</v>
+      </c>
+      <c r="J2160">
+        <v>0</v>
+      </c>
+      <c r="K2160">
+        <v>208</v>
+      </c>
+      <c r="L2160">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2161">
+        <v>2017</v>
+      </c>
+      <c r="B2161">
+        <v>3</v>
+      </c>
+      <c r="C2161" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2161" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2161">
+        <v>4</v>
+      </c>
+      <c r="F2161">
+        <v>68</v>
+      </c>
+      <c r="G2161">
+        <v>5</v>
+      </c>
+      <c r="H2161">
+        <v>85</v>
+      </c>
+      <c r="I2161">
+        <v>0</v>
+      </c>
+      <c r="J2161">
+        <v>0</v>
+      </c>
+      <c r="K2161">
+        <v>0</v>
+      </c>
+      <c r="L2161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2162">
+        <v>2017</v>
+      </c>
+      <c r="B2162">
+        <v>3</v>
+      </c>
+      <c r="C2162" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2162" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2162">
+        <v>2</v>
+      </c>
+      <c r="F2162">
+        <v>22</v>
+      </c>
+      <c r="G2162">
+        <v>7</v>
+      </c>
+      <c r="H2162">
+        <v>77</v>
+      </c>
+      <c r="I2162">
+        <v>0</v>
+      </c>
+      <c r="J2162">
+        <v>0</v>
+      </c>
+      <c r="K2162">
+        <v>4</v>
+      </c>
+      <c r="L2162">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2163">
+        <v>2017</v>
+      </c>
+      <c r="B2163">
+        <v>3</v>
+      </c>
+      <c r="C2163" s="1">
+        <v>820</v>
+      </c>
+      <c r="D2163" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2163">
+        <v>2</v>
+      </c>
+      <c r="F2163">
+        <v>22</v>
+      </c>
+      <c r="G2163">
+        <v>3</v>
+      </c>
+      <c r="H2163">
+        <v>33</v>
+      </c>
+      <c r="I2163">
+        <v>2</v>
+      </c>
+      <c r="J2163">
+        <v>22</v>
+      </c>
+      <c r="K2163">
+        <v>4</v>
+      </c>
+      <c r="L2163">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2164">
+        <v>2017</v>
+      </c>
+      <c r="B2164">
+        <v>3</v>
+      </c>
+      <c r="C2164" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2164" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2164">
+        <v>4406</v>
+      </c>
+      <c r="F2164">
+        <v>4406</v>
+      </c>
+      <c r="G2164">
+        <v>4840</v>
+      </c>
+      <c r="H2164">
+        <v>4840</v>
+      </c>
+      <c r="I2164">
+        <v>1790</v>
+      </c>
+      <c r="J2164">
+        <v>1790</v>
+      </c>
+      <c r="K2164">
+        <v>2335</v>
+      </c>
+      <c r="L2164">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2165">
+        <v>2017</v>
+      </c>
+      <c r="B2165">
+        <v>3</v>
+      </c>
+      <c r="C2165" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2165" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2165">
+        <v>0</v>
+      </c>
+      <c r="F2165">
+        <v>0</v>
+      </c>
+      <c r="G2165">
+        <v>3284</v>
+      </c>
+      <c r="H2165">
+        <v>9852</v>
+      </c>
+      <c r="I2165">
+        <v>-19</v>
+      </c>
+      <c r="J2165">
+        <v>-57</v>
+      </c>
+      <c r="K2165">
+        <v>2339</v>
+      </c>
+      <c r="L2165">
+        <v>7017</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2166">
+        <v>2017</v>
+      </c>
+      <c r="B2166">
+        <v>3</v>
+      </c>
+      <c r="C2166" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2166" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2166">
+        <v>124</v>
+      </c>
+      <c r="F2166">
+        <v>2108</v>
+      </c>
+      <c r="G2166">
+        <v>133</v>
+      </c>
+      <c r="H2166">
+        <v>2261</v>
+      </c>
+      <c r="I2166">
+        <v>76</v>
+      </c>
+      <c r="J2166">
+        <v>1292</v>
+      </c>
+      <c r="K2166">
+        <v>105</v>
+      </c>
+      <c r="L2166">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2167">
+        <v>2017</v>
+      </c>
+      <c r="B2167">
+        <v>3</v>
+      </c>
+      <c r="C2167" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2167" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2167">
+        <v>2</v>
+      </c>
+      <c r="F2167">
+        <v>22</v>
+      </c>
+      <c r="G2167">
+        <v>2</v>
+      </c>
+      <c r="H2167">
+        <v>22</v>
+      </c>
+      <c r="I2167">
+        <v>0</v>
+      </c>
+      <c r="J2167">
+        <v>0</v>
+      </c>
+      <c r="K2167">
+        <v>0</v>
+      </c>
+      <c r="L2167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2168">
+        <v>2017</v>
+      </c>
+      <c r="B2168">
+        <v>3</v>
+      </c>
+      <c r="C2168" s="1">
+        <v>860</v>
+      </c>
+      <c r="D2168" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2168">
+        <v>54</v>
+      </c>
+      <c r="F2168">
+        <v>54</v>
+      </c>
+      <c r="G2168">
+        <v>54</v>
+      </c>
+      <c r="H2168">
+        <v>54</v>
+      </c>
+      <c r="I2168">
+        <v>0</v>
+      </c>
+      <c r="J2168">
+        <v>0</v>
+      </c>
+      <c r="K2168">
+        <v>40</v>
+      </c>
+      <c r="L2168">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2169">
+        <v>2017</v>
+      </c>
+      <c r="B2169">
+        <v>3</v>
+      </c>
+      <c r="C2169" s="1">
+        <v>860</v>
+      </c>
+      <c r="D2169" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2169">
+        <v>0</v>
+      </c>
+      <c r="F2169">
+        <v>0</v>
+      </c>
+      <c r="G2169">
+        <v>48</v>
+      </c>
+      <c r="H2169">
+        <v>144</v>
+      </c>
+      <c r="I2169">
+        <v>0</v>
+      </c>
+      <c r="J2169">
+        <v>0</v>
+      </c>
+      <c r="K2169">
+        <v>36</v>
+      </c>
+      <c r="L2169">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Seeded Acres report data and Grain Shrink Additional Reports
</commit_message>
<xml_diff>
--- a/UploadedFiles/SeededAcres.xlsx
+++ b/UploadedFiles/SeededAcres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4357" uniqueCount="43">
   <si>
     <t>FiscalYear</t>
   </si>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2169" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2225" totalsRowShown="0">
   <tableColumns count="12">
     <tableColumn id="1" name="FiscalYear"/>
     <tableColumn id="2" name="FiscalPeriod"/>
@@ -308,6 +308,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -343,6 +360,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -495,11 +529,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2169"/>
+  <dimension ref="A1:L2225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2225" sqref="A2225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82936,6 +82970,2134 @@
         <v>108</v>
       </c>
     </row>
+    <row r="2170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2170">
+        <v>2017</v>
+      </c>
+      <c r="B2170">
+        <v>4</v>
+      </c>
+      <c r="C2170" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2170" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2170">
+        <v>20003</v>
+      </c>
+      <c r="F2170">
+        <v>20003</v>
+      </c>
+      <c r="G2170">
+        <v>22281</v>
+      </c>
+      <c r="H2170">
+        <v>22281</v>
+      </c>
+      <c r="I2170">
+        <v>12169</v>
+      </c>
+      <c r="J2170">
+        <v>12169</v>
+      </c>
+      <c r="K2170">
+        <v>13215</v>
+      </c>
+      <c r="L2170">
+        <v>13215</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2171">
+        <v>2017</v>
+      </c>
+      <c r="B2171">
+        <v>4</v>
+      </c>
+      <c r="C2171" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2171" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2171">
+        <v>44</v>
+      </c>
+      <c r="F2171">
+        <v>132</v>
+      </c>
+      <c r="G2171">
+        <v>853</v>
+      </c>
+      <c r="H2171">
+        <v>2559</v>
+      </c>
+      <c r="I2171">
+        <v>40</v>
+      </c>
+      <c r="J2171">
+        <v>120</v>
+      </c>
+      <c r="K2171">
+        <v>576</v>
+      </c>
+      <c r="L2171">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2172">
+        <v>2017</v>
+      </c>
+      <c r="B2172">
+        <v>4</v>
+      </c>
+      <c r="C2172" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2172" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2172">
+        <v>463</v>
+      </c>
+      <c r="F2172">
+        <v>7871</v>
+      </c>
+      <c r="G2172">
+        <v>501</v>
+      </c>
+      <c r="H2172">
+        <v>8517</v>
+      </c>
+      <c r="I2172">
+        <v>420</v>
+      </c>
+      <c r="J2172">
+        <v>7140</v>
+      </c>
+      <c r="K2172">
+        <v>457</v>
+      </c>
+      <c r="L2172">
+        <v>7769</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2173">
+        <v>2017</v>
+      </c>
+      <c r="B2173">
+        <v>4</v>
+      </c>
+      <c r="C2173" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2173" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2173">
+        <v>11</v>
+      </c>
+      <c r="F2173">
+        <v>121</v>
+      </c>
+      <c r="G2173">
+        <v>33</v>
+      </c>
+      <c r="H2173">
+        <v>363</v>
+      </c>
+      <c r="I2173">
+        <v>12</v>
+      </c>
+      <c r="J2173">
+        <v>132</v>
+      </c>
+      <c r="K2173">
+        <v>50</v>
+      </c>
+      <c r="L2173">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2174">
+        <v>2017</v>
+      </c>
+      <c r="B2174">
+        <v>4</v>
+      </c>
+      <c r="C2174" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2174" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2174">
+        <v>0</v>
+      </c>
+      <c r="F2174">
+        <v>0</v>
+      </c>
+      <c r="G2174">
+        <v>0</v>
+      </c>
+      <c r="H2174">
+        <v>0</v>
+      </c>
+      <c r="I2174">
+        <v>23</v>
+      </c>
+      <c r="J2174">
+        <v>23</v>
+      </c>
+      <c r="K2174">
+        <v>23</v>
+      </c>
+      <c r="L2174">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2175">
+        <v>2017</v>
+      </c>
+      <c r="B2175">
+        <v>4</v>
+      </c>
+      <c r="C2175" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2175" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2175">
+        <v>0</v>
+      </c>
+      <c r="F2175">
+        <v>0</v>
+      </c>
+      <c r="G2175">
+        <v>13</v>
+      </c>
+      <c r="H2175">
+        <v>39</v>
+      </c>
+      <c r="I2175">
+        <v>-3</v>
+      </c>
+      <c r="J2175">
+        <v>-9</v>
+      </c>
+      <c r="K2175">
+        <v>74</v>
+      </c>
+      <c r="L2175">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2176">
+        <v>2017</v>
+      </c>
+      <c r="B2176">
+        <v>4</v>
+      </c>
+      <c r="C2176" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2176" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2176">
+        <v>15</v>
+      </c>
+      <c r="F2176">
+        <v>255</v>
+      </c>
+      <c r="G2176">
+        <v>15</v>
+      </c>
+      <c r="H2176">
+        <v>255</v>
+      </c>
+      <c r="I2176">
+        <v>15</v>
+      </c>
+      <c r="J2176">
+        <v>255</v>
+      </c>
+      <c r="K2176">
+        <v>15</v>
+      </c>
+      <c r="L2176">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2177">
+        <v>2017</v>
+      </c>
+      <c r="B2177">
+        <v>4</v>
+      </c>
+      <c r="C2177" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2177" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2177">
+        <v>0</v>
+      </c>
+      <c r="F2177">
+        <v>0</v>
+      </c>
+      <c r="G2177">
+        <v>3</v>
+      </c>
+      <c r="H2177">
+        <v>33</v>
+      </c>
+      <c r="I2177">
+        <v>0</v>
+      </c>
+      <c r="J2177">
+        <v>0</v>
+      </c>
+      <c r="K2177">
+        <v>2</v>
+      </c>
+      <c r="L2177">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2178">
+        <v>2017</v>
+      </c>
+      <c r="B2178">
+        <v>4</v>
+      </c>
+      <c r="C2178" s="1">
+        <v>140</v>
+      </c>
+      <c r="D2178" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2178">
+        <v>-5</v>
+      </c>
+      <c r="F2178">
+        <v>-85</v>
+      </c>
+      <c r="G2178">
+        <v>34</v>
+      </c>
+      <c r="H2178">
+        <v>578</v>
+      </c>
+      <c r="I2178">
+        <v>58</v>
+      </c>
+      <c r="J2178">
+        <v>986</v>
+      </c>
+      <c r="K2178">
+        <v>58</v>
+      </c>
+      <c r="L2178">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="2179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2179">
+        <v>2017</v>
+      </c>
+      <c r="B2179">
+        <v>4</v>
+      </c>
+      <c r="C2179" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2179" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2179">
+        <v>4862</v>
+      </c>
+      <c r="F2179">
+        <v>4862</v>
+      </c>
+      <c r="G2179">
+        <v>7622</v>
+      </c>
+      <c r="H2179">
+        <v>7622</v>
+      </c>
+      <c r="I2179">
+        <v>0</v>
+      </c>
+      <c r="J2179">
+        <v>0</v>
+      </c>
+      <c r="K2179">
+        <v>0</v>
+      </c>
+      <c r="L2179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2180">
+        <v>2017</v>
+      </c>
+      <c r="B2180">
+        <v>4</v>
+      </c>
+      <c r="C2180" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2180" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2180">
+        <v>-14</v>
+      </c>
+      <c r="F2180">
+        <v>-42</v>
+      </c>
+      <c r="G2180">
+        <v>213</v>
+      </c>
+      <c r="H2180">
+        <v>639</v>
+      </c>
+      <c r="I2180">
+        <v>3</v>
+      </c>
+      <c r="J2180">
+        <v>9</v>
+      </c>
+      <c r="K2180">
+        <v>203</v>
+      </c>
+      <c r="L2180">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2181">
+        <v>2017</v>
+      </c>
+      <c r="B2181">
+        <v>4</v>
+      </c>
+      <c r="C2181" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2181" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2181">
+        <v>27</v>
+      </c>
+      <c r="F2181">
+        <v>459</v>
+      </c>
+      <c r="G2181">
+        <v>27</v>
+      </c>
+      <c r="H2181">
+        <v>459</v>
+      </c>
+      <c r="I2181">
+        <v>4</v>
+      </c>
+      <c r="J2181">
+        <v>68</v>
+      </c>
+      <c r="K2181">
+        <v>7</v>
+      </c>
+      <c r="L2181">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2182">
+        <v>2017</v>
+      </c>
+      <c r="B2182">
+        <v>4</v>
+      </c>
+      <c r="C2182" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2182" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2182">
+        <v>0</v>
+      </c>
+      <c r="F2182">
+        <v>0</v>
+      </c>
+      <c r="G2182">
+        <v>2</v>
+      </c>
+      <c r="H2182">
+        <v>22</v>
+      </c>
+      <c r="I2182">
+        <v>1</v>
+      </c>
+      <c r="J2182">
+        <v>11</v>
+      </c>
+      <c r="K2182">
+        <v>3</v>
+      </c>
+      <c r="L2182">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2183">
+        <v>2017</v>
+      </c>
+      <c r="B2183">
+        <v>4</v>
+      </c>
+      <c r="C2183" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2183" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2183">
+        <v>40</v>
+      </c>
+      <c r="F2183">
+        <v>40</v>
+      </c>
+      <c r="G2183">
+        <v>40</v>
+      </c>
+      <c r="H2183">
+        <v>40</v>
+      </c>
+      <c r="I2183">
+        <v>80</v>
+      </c>
+      <c r="J2183">
+        <v>80</v>
+      </c>
+      <c r="K2183">
+        <v>80</v>
+      </c>
+      <c r="L2183">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2184">
+        <v>2017</v>
+      </c>
+      <c r="B2184">
+        <v>4</v>
+      </c>
+      <c r="C2184" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2184" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2184">
+        <v>0</v>
+      </c>
+      <c r="F2184">
+        <v>0</v>
+      </c>
+      <c r="G2184">
+        <v>69</v>
+      </c>
+      <c r="H2184">
+        <v>207</v>
+      </c>
+      <c r="I2184">
+        <v>0</v>
+      </c>
+      <c r="J2184">
+        <v>0</v>
+      </c>
+      <c r="K2184">
+        <v>94</v>
+      </c>
+      <c r="L2184">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2185">
+        <v>2017</v>
+      </c>
+      <c r="B2185">
+        <v>4</v>
+      </c>
+      <c r="C2185" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2185" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2185">
+        <v>3</v>
+      </c>
+      <c r="F2185">
+        <v>51</v>
+      </c>
+      <c r="G2185">
+        <v>9</v>
+      </c>
+      <c r="H2185">
+        <v>153</v>
+      </c>
+      <c r="I2185">
+        <v>0</v>
+      </c>
+      <c r="J2185">
+        <v>0</v>
+      </c>
+      <c r="K2185">
+        <v>0</v>
+      </c>
+      <c r="L2185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2186">
+        <v>2017</v>
+      </c>
+      <c r="B2186">
+        <v>4</v>
+      </c>
+      <c r="C2186" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2186" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2186">
+        <v>3</v>
+      </c>
+      <c r="F2186">
+        <v>33</v>
+      </c>
+      <c r="G2186">
+        <v>8</v>
+      </c>
+      <c r="H2186">
+        <v>88</v>
+      </c>
+      <c r="I2186">
+        <v>2</v>
+      </c>
+      <c r="J2186">
+        <v>22</v>
+      </c>
+      <c r="K2186">
+        <v>7</v>
+      </c>
+      <c r="L2186">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2187">
+        <v>2017</v>
+      </c>
+      <c r="B2187">
+        <v>4</v>
+      </c>
+      <c r="C2187" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2187" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2187">
+        <v>45</v>
+      </c>
+      <c r="F2187">
+        <v>45</v>
+      </c>
+      <c r="G2187">
+        <v>45</v>
+      </c>
+      <c r="H2187">
+        <v>45</v>
+      </c>
+      <c r="I2187">
+        <v>0</v>
+      </c>
+      <c r="J2187">
+        <v>0</v>
+      </c>
+      <c r="K2187">
+        <v>0</v>
+      </c>
+      <c r="L2187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2188">
+        <v>2017</v>
+      </c>
+      <c r="B2188">
+        <v>4</v>
+      </c>
+      <c r="C2188" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2188" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2188">
+        <v>0</v>
+      </c>
+      <c r="F2188">
+        <v>0</v>
+      </c>
+      <c r="G2188">
+        <v>184</v>
+      </c>
+      <c r="H2188">
+        <v>552</v>
+      </c>
+      <c r="I2188">
+        <v>0</v>
+      </c>
+      <c r="J2188">
+        <v>0</v>
+      </c>
+      <c r="K2188">
+        <v>93</v>
+      </c>
+      <c r="L2188">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2189">
+        <v>2017</v>
+      </c>
+      <c r="B2189">
+        <v>4</v>
+      </c>
+      <c r="C2189" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2189" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2189">
+        <v>11</v>
+      </c>
+      <c r="F2189">
+        <v>187</v>
+      </c>
+      <c r="G2189">
+        <v>11</v>
+      </c>
+      <c r="H2189">
+        <v>187</v>
+      </c>
+      <c r="I2189">
+        <v>56</v>
+      </c>
+      <c r="J2189">
+        <v>952</v>
+      </c>
+      <c r="K2189">
+        <v>56</v>
+      </c>
+      <c r="L2189">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="2190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2190">
+        <v>2017</v>
+      </c>
+      <c r="B2190">
+        <v>4</v>
+      </c>
+      <c r="C2190" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2190" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2190">
+        <v>2</v>
+      </c>
+      <c r="F2190">
+        <v>22</v>
+      </c>
+      <c r="G2190">
+        <v>9</v>
+      </c>
+      <c r="H2190">
+        <v>99</v>
+      </c>
+      <c r="I2190">
+        <v>0</v>
+      </c>
+      <c r="J2190">
+        <v>0</v>
+      </c>
+      <c r="K2190">
+        <v>10</v>
+      </c>
+      <c r="L2190">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2191">
+        <v>2017</v>
+      </c>
+      <c r="B2191">
+        <v>4</v>
+      </c>
+      <c r="C2191" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2191" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2191">
+        <v>14245</v>
+      </c>
+      <c r="F2191">
+        <v>14245</v>
+      </c>
+      <c r="G2191">
+        <v>21153</v>
+      </c>
+      <c r="H2191">
+        <v>21153</v>
+      </c>
+      <c r="I2191">
+        <v>18649</v>
+      </c>
+      <c r="J2191">
+        <v>18649</v>
+      </c>
+      <c r="K2191">
+        <v>23664</v>
+      </c>
+      <c r="L2191">
+        <v>23664</v>
+      </c>
+    </row>
+    <row r="2192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2192">
+        <v>2017</v>
+      </c>
+      <c r="B2192">
+        <v>4</v>
+      </c>
+      <c r="C2192" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2192" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2192">
+        <v>73</v>
+      </c>
+      <c r="F2192">
+        <v>219</v>
+      </c>
+      <c r="G2192">
+        <v>4504</v>
+      </c>
+      <c r="H2192">
+        <v>13512</v>
+      </c>
+      <c r="I2192">
+        <v>72</v>
+      </c>
+      <c r="J2192">
+        <v>216</v>
+      </c>
+      <c r="K2192">
+        <v>4093</v>
+      </c>
+      <c r="L2192">
+        <v>12279</v>
+      </c>
+    </row>
+    <row r="2193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2193">
+        <v>2017</v>
+      </c>
+      <c r="B2193">
+        <v>4</v>
+      </c>
+      <c r="C2193" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2193" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2193">
+        <v>430</v>
+      </c>
+      <c r="F2193">
+        <v>7310</v>
+      </c>
+      <c r="G2193">
+        <v>1073</v>
+      </c>
+      <c r="H2193">
+        <v>18241</v>
+      </c>
+      <c r="I2193">
+        <v>417</v>
+      </c>
+      <c r="J2193">
+        <v>7089</v>
+      </c>
+      <c r="K2193">
+        <v>767</v>
+      </c>
+      <c r="L2193">
+        <v>13039</v>
+      </c>
+    </row>
+    <row r="2194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2194">
+        <v>2017</v>
+      </c>
+      <c r="B2194">
+        <v>4</v>
+      </c>
+      <c r="C2194" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2194" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2194">
+        <v>6313</v>
+      </c>
+      <c r="F2194">
+        <v>6313</v>
+      </c>
+      <c r="G2194">
+        <v>7596</v>
+      </c>
+      <c r="H2194">
+        <v>7596</v>
+      </c>
+      <c r="I2194">
+        <v>8420</v>
+      </c>
+      <c r="J2194">
+        <v>8420</v>
+      </c>
+      <c r="K2194">
+        <v>11135</v>
+      </c>
+      <c r="L2194">
+        <v>11135</v>
+      </c>
+    </row>
+    <row r="2195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2195">
+        <v>2017</v>
+      </c>
+      <c r="B2195">
+        <v>4</v>
+      </c>
+      <c r="C2195" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2195" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2195">
+        <v>14</v>
+      </c>
+      <c r="F2195">
+        <v>42</v>
+      </c>
+      <c r="G2195">
+        <v>2754</v>
+      </c>
+      <c r="H2195">
+        <v>8262</v>
+      </c>
+      <c r="I2195">
+        <v>19</v>
+      </c>
+      <c r="J2195">
+        <v>57</v>
+      </c>
+      <c r="K2195">
+        <v>2720</v>
+      </c>
+      <c r="L2195">
+        <v>8160</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2196">
+        <v>2017</v>
+      </c>
+      <c r="B2196">
+        <v>4</v>
+      </c>
+      <c r="C2196" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2196" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2196">
+        <v>426</v>
+      </c>
+      <c r="F2196">
+        <v>7242</v>
+      </c>
+      <c r="G2196">
+        <v>555</v>
+      </c>
+      <c r="H2196">
+        <v>9435</v>
+      </c>
+      <c r="I2196">
+        <v>506</v>
+      </c>
+      <c r="J2196">
+        <v>8602</v>
+      </c>
+      <c r="K2196">
+        <v>608</v>
+      </c>
+      <c r="L2196">
+        <v>10336</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2197">
+        <v>2017</v>
+      </c>
+      <c r="B2197">
+        <v>4</v>
+      </c>
+      <c r="C2197" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2197" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2197">
+        <v>5377</v>
+      </c>
+      <c r="F2197">
+        <v>5377</v>
+      </c>
+      <c r="G2197">
+        <v>8808</v>
+      </c>
+      <c r="H2197">
+        <v>8808</v>
+      </c>
+      <c r="I2197">
+        <v>5450</v>
+      </c>
+      <c r="J2197">
+        <v>5450</v>
+      </c>
+      <c r="K2197">
+        <v>6577</v>
+      </c>
+      <c r="L2197">
+        <v>6577</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2198">
+        <v>2017</v>
+      </c>
+      <c r="B2198">
+        <v>4</v>
+      </c>
+      <c r="C2198" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2198" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2198">
+        <v>27</v>
+      </c>
+      <c r="F2198">
+        <v>81</v>
+      </c>
+      <c r="G2198">
+        <v>1183</v>
+      </c>
+      <c r="H2198">
+        <v>3549</v>
+      </c>
+      <c r="I2198">
+        <v>-5</v>
+      </c>
+      <c r="J2198">
+        <v>-15</v>
+      </c>
+      <c r="K2198">
+        <v>917</v>
+      </c>
+      <c r="L2198">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2199">
+        <v>2017</v>
+      </c>
+      <c r="B2199">
+        <v>4</v>
+      </c>
+      <c r="C2199" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2199" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2199">
+        <v>1052</v>
+      </c>
+      <c r="F2199">
+        <v>17884</v>
+      </c>
+      <c r="G2199">
+        <v>1327</v>
+      </c>
+      <c r="H2199">
+        <v>22559</v>
+      </c>
+      <c r="I2199">
+        <v>1078</v>
+      </c>
+      <c r="J2199">
+        <v>18326</v>
+      </c>
+      <c r="K2199">
+        <v>1301</v>
+      </c>
+      <c r="L2199">
+        <v>22117</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2200">
+        <v>2017</v>
+      </c>
+      <c r="B2200">
+        <v>4</v>
+      </c>
+      <c r="C2200" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2200" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2200">
+        <v>4</v>
+      </c>
+      <c r="F2200">
+        <v>44</v>
+      </c>
+      <c r="G2200">
+        <v>8</v>
+      </c>
+      <c r="H2200">
+        <v>88</v>
+      </c>
+      <c r="I2200">
+        <v>1</v>
+      </c>
+      <c r="J2200">
+        <v>11</v>
+      </c>
+      <c r="K2200">
+        <v>9</v>
+      </c>
+      <c r="L2200">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2201">
+        <v>2017</v>
+      </c>
+      <c r="B2201">
+        <v>4</v>
+      </c>
+      <c r="C2201" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2201" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2201">
+        <v>4076</v>
+      </c>
+      <c r="F2201">
+        <v>4076</v>
+      </c>
+      <c r="G2201">
+        <v>9945</v>
+      </c>
+      <c r="H2201">
+        <v>9945</v>
+      </c>
+      <c r="I2201">
+        <v>7203</v>
+      </c>
+      <c r="J2201">
+        <v>7203</v>
+      </c>
+      <c r="K2201">
+        <v>10346</v>
+      </c>
+      <c r="L2201">
+        <v>10346</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2202">
+        <v>2017</v>
+      </c>
+      <c r="B2202">
+        <v>4</v>
+      </c>
+      <c r="C2202" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2202" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2202">
+        <v>-16</v>
+      </c>
+      <c r="F2202">
+        <v>-48</v>
+      </c>
+      <c r="G2202">
+        <v>2139</v>
+      </c>
+      <c r="H2202">
+        <v>6417</v>
+      </c>
+      <c r="I2202">
+        <v>1</v>
+      </c>
+      <c r="J2202">
+        <v>3</v>
+      </c>
+      <c r="K2202">
+        <v>1890</v>
+      </c>
+      <c r="L2202">
+        <v>5670</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2203">
+        <v>2017</v>
+      </c>
+      <c r="B2203">
+        <v>4</v>
+      </c>
+      <c r="C2203" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2203" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2203">
+        <v>82</v>
+      </c>
+      <c r="F2203">
+        <v>1394</v>
+      </c>
+      <c r="G2203">
+        <v>126</v>
+      </c>
+      <c r="H2203">
+        <v>2142</v>
+      </c>
+      <c r="I2203">
+        <v>90</v>
+      </c>
+      <c r="J2203">
+        <v>1530</v>
+      </c>
+      <c r="K2203">
+        <v>134</v>
+      </c>
+      <c r="L2203">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2204">
+        <v>2017</v>
+      </c>
+      <c r="B2204">
+        <v>4</v>
+      </c>
+      <c r="C2204" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2204" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2204">
+        <v>4</v>
+      </c>
+      <c r="F2204">
+        <v>44</v>
+      </c>
+      <c r="G2204">
+        <v>27</v>
+      </c>
+      <c r="H2204">
+        <v>306</v>
+      </c>
+      <c r="I2204">
+        <v>2</v>
+      </c>
+      <c r="J2204">
+        <v>30</v>
+      </c>
+      <c r="K2204">
+        <v>23</v>
+      </c>
+      <c r="L2204">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2205">
+        <v>2017</v>
+      </c>
+      <c r="B2205">
+        <v>4</v>
+      </c>
+      <c r="C2205" s="1">
+        <v>580</v>
+      </c>
+      <c r="D2205" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2205">
+        <v>16</v>
+      </c>
+      <c r="F2205">
+        <v>16</v>
+      </c>
+      <c r="G2205">
+        <v>16</v>
+      </c>
+      <c r="H2205">
+        <v>16</v>
+      </c>
+      <c r="I2205">
+        <v>29</v>
+      </c>
+      <c r="J2205">
+        <v>29</v>
+      </c>
+      <c r="K2205">
+        <v>29</v>
+      </c>
+      <c r="L2205">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2206">
+        <v>2017</v>
+      </c>
+      <c r="B2206">
+        <v>4</v>
+      </c>
+      <c r="C2206" s="1">
+        <v>580</v>
+      </c>
+      <c r="D2206" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2206">
+        <v>0</v>
+      </c>
+      <c r="F2206">
+        <v>0</v>
+      </c>
+      <c r="G2206">
+        <v>-2</v>
+      </c>
+      <c r="H2206">
+        <v>-6</v>
+      </c>
+      <c r="I2206">
+        <v>0</v>
+      </c>
+      <c r="J2206">
+        <v>0</v>
+      </c>
+      <c r="K2206">
+        <v>0</v>
+      </c>
+      <c r="L2206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2207">
+        <v>2017</v>
+      </c>
+      <c r="B2207">
+        <v>4</v>
+      </c>
+      <c r="C2207" s="1">
+        <v>580</v>
+      </c>
+      <c r="D2207" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2207">
+        <v>2</v>
+      </c>
+      <c r="F2207">
+        <v>34</v>
+      </c>
+      <c r="G2207">
+        <v>2</v>
+      </c>
+      <c r="H2207">
+        <v>34</v>
+      </c>
+      <c r="I2207">
+        <v>24</v>
+      </c>
+      <c r="J2207">
+        <v>408</v>
+      </c>
+      <c r="K2207">
+        <v>24</v>
+      </c>
+      <c r="L2207">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2208">
+        <v>2017</v>
+      </c>
+      <c r="B2208">
+        <v>4</v>
+      </c>
+      <c r="C2208" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2208" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2208">
+        <v>0</v>
+      </c>
+      <c r="F2208">
+        <v>0</v>
+      </c>
+      <c r="G2208">
+        <v>140</v>
+      </c>
+      <c r="H2208">
+        <v>140</v>
+      </c>
+      <c r="I2208">
+        <v>0</v>
+      </c>
+      <c r="J2208">
+        <v>0</v>
+      </c>
+      <c r="K2208">
+        <v>0</v>
+      </c>
+      <c r="L2208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2209">
+        <v>2017</v>
+      </c>
+      <c r="B2209">
+        <v>4</v>
+      </c>
+      <c r="C2209" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2209" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2209">
+        <v>0</v>
+      </c>
+      <c r="F2209">
+        <v>0</v>
+      </c>
+      <c r="G2209">
+        <v>4</v>
+      </c>
+      <c r="H2209">
+        <v>12</v>
+      </c>
+      <c r="I2209">
+        <v>0</v>
+      </c>
+      <c r="J2209">
+        <v>0</v>
+      </c>
+      <c r="K2209">
+        <v>1</v>
+      </c>
+      <c r="L2209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2210">
+        <v>2017</v>
+      </c>
+      <c r="B2210">
+        <v>4</v>
+      </c>
+      <c r="C2210" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2210" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2210">
+        <v>0</v>
+      </c>
+      <c r="F2210">
+        <v>0</v>
+      </c>
+      <c r="G2210">
+        <v>-1</v>
+      </c>
+      <c r="H2210">
+        <v>-17</v>
+      </c>
+      <c r="I2210">
+        <v>0</v>
+      </c>
+      <c r="J2210">
+        <v>0</v>
+      </c>
+      <c r="K2210">
+        <v>0</v>
+      </c>
+      <c r="L2210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2211">
+        <v>2017</v>
+      </c>
+      <c r="B2211">
+        <v>4</v>
+      </c>
+      <c r="C2211" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2211" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2211">
+        <v>1</v>
+      </c>
+      <c r="F2211">
+        <v>11</v>
+      </c>
+      <c r="G2211">
+        <v>6</v>
+      </c>
+      <c r="H2211">
+        <v>66</v>
+      </c>
+      <c r="I2211">
+        <v>2</v>
+      </c>
+      <c r="J2211">
+        <v>22</v>
+      </c>
+      <c r="K2211">
+        <v>4</v>
+      </c>
+      <c r="L2211">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2212">
+        <v>2017</v>
+      </c>
+      <c r="B2212">
+        <v>4</v>
+      </c>
+      <c r="C2212" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2212" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2212">
+        <v>147</v>
+      </c>
+      <c r="F2212">
+        <v>147</v>
+      </c>
+      <c r="G2212">
+        <v>210</v>
+      </c>
+      <c r="H2212">
+        <v>210</v>
+      </c>
+      <c r="I2212">
+        <v>164</v>
+      </c>
+      <c r="J2212">
+        <v>164</v>
+      </c>
+      <c r="K2212">
+        <v>194</v>
+      </c>
+      <c r="L2212">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2213">
+        <v>2017</v>
+      </c>
+      <c r="B2213">
+        <v>4</v>
+      </c>
+      <c r="C2213" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2213" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2213">
+        <v>-3</v>
+      </c>
+      <c r="F2213">
+        <v>-9</v>
+      </c>
+      <c r="G2213">
+        <v>209</v>
+      </c>
+      <c r="H2213">
+        <v>627</v>
+      </c>
+      <c r="I2213">
+        <v>-3</v>
+      </c>
+      <c r="J2213">
+        <v>-9</v>
+      </c>
+      <c r="K2213">
+        <v>272</v>
+      </c>
+      <c r="L2213">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2214">
+        <v>2017</v>
+      </c>
+      <c r="B2214">
+        <v>4</v>
+      </c>
+      <c r="C2214" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2214" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2214">
+        <v>49</v>
+      </c>
+      <c r="F2214">
+        <v>833</v>
+      </c>
+      <c r="G2214">
+        <v>49</v>
+      </c>
+      <c r="H2214">
+        <v>833</v>
+      </c>
+      <c r="I2214">
+        <v>10</v>
+      </c>
+      <c r="J2214">
+        <v>170</v>
+      </c>
+      <c r="K2214">
+        <v>13</v>
+      </c>
+      <c r="L2214">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2215">
+        <v>2017</v>
+      </c>
+      <c r="B2215">
+        <v>4</v>
+      </c>
+      <c r="C2215" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2215" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2215">
+        <v>0</v>
+      </c>
+      <c r="F2215">
+        <v>0</v>
+      </c>
+      <c r="G2215">
+        <v>2</v>
+      </c>
+      <c r="H2215">
+        <v>22</v>
+      </c>
+      <c r="I2215">
+        <v>1</v>
+      </c>
+      <c r="J2215">
+        <v>11</v>
+      </c>
+      <c r="K2215">
+        <v>4</v>
+      </c>
+      <c r="L2215">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2216">
+        <v>2017</v>
+      </c>
+      <c r="B2216">
+        <v>4</v>
+      </c>
+      <c r="C2216" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2216" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2216">
+        <v>0</v>
+      </c>
+      <c r="F2216">
+        <v>0</v>
+      </c>
+      <c r="G2216">
+        <v>0</v>
+      </c>
+      <c r="H2216">
+        <v>0</v>
+      </c>
+      <c r="I2216">
+        <v>54</v>
+      </c>
+      <c r="J2216">
+        <v>54</v>
+      </c>
+      <c r="K2216">
+        <v>54</v>
+      </c>
+      <c r="L2216">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2217">
+        <v>2017</v>
+      </c>
+      <c r="B2217">
+        <v>4</v>
+      </c>
+      <c r="C2217" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2217" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2217">
+        <v>0</v>
+      </c>
+      <c r="F2217">
+        <v>0</v>
+      </c>
+      <c r="G2217">
+        <v>499</v>
+      </c>
+      <c r="H2217">
+        <v>1497</v>
+      </c>
+      <c r="I2217">
+        <v>0</v>
+      </c>
+      <c r="J2217">
+        <v>0</v>
+      </c>
+      <c r="K2217">
+        <v>208</v>
+      </c>
+      <c r="L2217">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2218">
+        <v>2017</v>
+      </c>
+      <c r="B2218">
+        <v>4</v>
+      </c>
+      <c r="C2218" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2218" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2218">
+        <v>12</v>
+      </c>
+      <c r="F2218">
+        <v>204</v>
+      </c>
+      <c r="G2218">
+        <v>17</v>
+      </c>
+      <c r="H2218">
+        <v>289</v>
+      </c>
+      <c r="I2218">
+        <v>46</v>
+      </c>
+      <c r="J2218">
+        <v>782</v>
+      </c>
+      <c r="K2218">
+        <v>46</v>
+      </c>
+      <c r="L2218">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2219">
+        <v>2017</v>
+      </c>
+      <c r="B2219">
+        <v>4</v>
+      </c>
+      <c r="C2219" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2219" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2219">
+        <v>1</v>
+      </c>
+      <c r="F2219">
+        <v>11</v>
+      </c>
+      <c r="G2219">
+        <v>8</v>
+      </c>
+      <c r="H2219">
+        <v>88</v>
+      </c>
+      <c r="I2219">
+        <v>4</v>
+      </c>
+      <c r="J2219">
+        <v>44</v>
+      </c>
+      <c r="K2219">
+        <v>8</v>
+      </c>
+      <c r="L2219">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2220">
+        <v>2017</v>
+      </c>
+      <c r="B2220">
+        <v>4</v>
+      </c>
+      <c r="C2220" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2220" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2220">
+        <v>10665</v>
+      </c>
+      <c r="F2220">
+        <v>10665</v>
+      </c>
+      <c r="G2220">
+        <v>15506</v>
+      </c>
+      <c r="H2220">
+        <v>15506</v>
+      </c>
+      <c r="I2220">
+        <v>14641</v>
+      </c>
+      <c r="J2220">
+        <v>14641</v>
+      </c>
+      <c r="K2220">
+        <v>16977</v>
+      </c>
+      <c r="L2220">
+        <v>16977</v>
+      </c>
+    </row>
+    <row r="2221" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2221">
+        <v>2017</v>
+      </c>
+      <c r="B2221">
+        <v>4</v>
+      </c>
+      <c r="C2221" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2221" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2221">
+        <v>33</v>
+      </c>
+      <c r="F2221">
+        <v>99</v>
+      </c>
+      <c r="G2221">
+        <v>3317</v>
+      </c>
+      <c r="H2221">
+        <v>9951</v>
+      </c>
+      <c r="I2221">
+        <v>-32</v>
+      </c>
+      <c r="J2221">
+        <v>-96</v>
+      </c>
+      <c r="K2221">
+        <v>2307</v>
+      </c>
+      <c r="L2221">
+        <v>6921</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2222">
+        <v>2017</v>
+      </c>
+      <c r="B2222">
+        <v>4</v>
+      </c>
+      <c r="C2222" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2222" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2222">
+        <v>168</v>
+      </c>
+      <c r="F2222">
+        <v>2856</v>
+      </c>
+      <c r="G2222">
+        <v>301</v>
+      </c>
+      <c r="H2222">
+        <v>5117</v>
+      </c>
+      <c r="I2222">
+        <v>311</v>
+      </c>
+      <c r="J2222">
+        <v>5287</v>
+      </c>
+      <c r="K2222">
+        <v>416</v>
+      </c>
+      <c r="L2222">
+        <v>7072</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2223">
+        <v>2017</v>
+      </c>
+      <c r="B2223">
+        <v>4</v>
+      </c>
+      <c r="C2223" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2223" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2223">
+        <v>0</v>
+      </c>
+      <c r="F2223">
+        <v>0</v>
+      </c>
+      <c r="G2223">
+        <v>2</v>
+      </c>
+      <c r="H2223">
+        <v>22</v>
+      </c>
+      <c r="I2223">
+        <v>0</v>
+      </c>
+      <c r="J2223">
+        <v>0</v>
+      </c>
+      <c r="K2223">
+        <v>0</v>
+      </c>
+      <c r="L2223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2224">
+        <v>2017</v>
+      </c>
+      <c r="B2224">
+        <v>4</v>
+      </c>
+      <c r="C2224" s="1">
+        <v>860</v>
+      </c>
+      <c r="D2224" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2224">
+        <v>276</v>
+      </c>
+      <c r="F2224">
+        <v>276</v>
+      </c>
+      <c r="G2224">
+        <v>330</v>
+      </c>
+      <c r="H2224">
+        <v>330</v>
+      </c>
+      <c r="I2224">
+        <v>147</v>
+      </c>
+      <c r="J2224">
+        <v>147</v>
+      </c>
+      <c r="K2224">
+        <v>187</v>
+      </c>
+      <c r="L2224">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2225">
+        <v>2017</v>
+      </c>
+      <c r="B2225">
+        <v>4</v>
+      </c>
+      <c r="C2225" s="1">
+        <v>860</v>
+      </c>
+      <c r="D2225" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2225">
+        <v>0</v>
+      </c>
+      <c r="F2225">
+        <v>0</v>
+      </c>
+      <c r="G2225">
+        <v>48</v>
+      </c>
+      <c r="H2225">
+        <v>144</v>
+      </c>
+      <c r="I2225">
+        <v>0</v>
+      </c>
+      <c r="J2225">
+        <v>0</v>
+      </c>
+      <c r="K2225">
+        <v>36</v>
+      </c>
+      <c r="L2225">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Plan highlight, hid Seeded Acres tab, updated location data
</commit_message>
<xml_diff>
--- a/UploadedFiles/SeededAcres.xlsx
+++ b/UploadedFiles/SeededAcres.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="SeededAcres" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4357" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4409" uniqueCount="43">
   <si>
     <t>FiscalYear</t>
   </si>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2225" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSeededAcres" displayName="tblSeededAcres" ref="A1:L2276" totalsRowShown="0">
   <tableColumns count="12">
     <tableColumn id="1" name="FiscalYear"/>
     <tableColumn id="2" name="FiscalPeriod"/>
@@ -529,11 +529,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2225"/>
+  <dimension ref="A1:L2276"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2225" sqref="A2225"/>
+      <pane ySplit="1" topLeftCell="A2248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2276" sqref="A2276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85098,6 +85098,1944 @@
         <v>108</v>
       </c>
     </row>
+    <row r="2226" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2226">
+        <v>2017</v>
+      </c>
+      <c r="B2226">
+        <v>5</v>
+      </c>
+      <c r="C2226" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2226" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2226">
+        <v>743</v>
+      </c>
+      <c r="F2226">
+        <v>743</v>
+      </c>
+      <c r="G2226">
+        <v>23024</v>
+      </c>
+      <c r="H2226">
+        <v>23024</v>
+      </c>
+      <c r="I2226">
+        <v>1305</v>
+      </c>
+      <c r="J2226">
+        <v>1305</v>
+      </c>
+      <c r="K2226">
+        <v>14520</v>
+      </c>
+      <c r="L2226">
+        <v>14520</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2227">
+        <v>2017</v>
+      </c>
+      <c r="B2227">
+        <v>5</v>
+      </c>
+      <c r="C2227" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2227" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2227">
+        <v>-42</v>
+      </c>
+      <c r="F2227">
+        <v>-126</v>
+      </c>
+      <c r="G2227">
+        <v>811</v>
+      </c>
+      <c r="H2227">
+        <v>2433</v>
+      </c>
+      <c r="I2227">
+        <v>38</v>
+      </c>
+      <c r="J2227">
+        <v>114</v>
+      </c>
+      <c r="K2227">
+        <v>614</v>
+      </c>
+      <c r="L2227">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2228">
+        <v>2017</v>
+      </c>
+      <c r="B2228">
+        <v>5</v>
+      </c>
+      <c r="C2228" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2228" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2228">
+        <v>0</v>
+      </c>
+      <c r="F2228">
+        <v>0</v>
+      </c>
+      <c r="G2228">
+        <v>501</v>
+      </c>
+      <c r="H2228">
+        <v>8517</v>
+      </c>
+      <c r="I2228">
+        <v>1</v>
+      </c>
+      <c r="J2228">
+        <v>17</v>
+      </c>
+      <c r="K2228">
+        <v>458</v>
+      </c>
+      <c r="L2228">
+        <v>7786</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2229">
+        <v>2017</v>
+      </c>
+      <c r="B2229">
+        <v>5</v>
+      </c>
+      <c r="C2229" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2229" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2229">
+        <v>5</v>
+      </c>
+      <c r="F2229">
+        <v>55</v>
+      </c>
+      <c r="G2229">
+        <v>38</v>
+      </c>
+      <c r="H2229">
+        <v>418</v>
+      </c>
+      <c r="I2229">
+        <v>9</v>
+      </c>
+      <c r="J2229">
+        <v>99</v>
+      </c>
+      <c r="K2229">
+        <v>59</v>
+      </c>
+      <c r="L2229">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2230">
+        <v>2017</v>
+      </c>
+      <c r="B2230">
+        <v>5</v>
+      </c>
+      <c r="C2230" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2230" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2230">
+        <v>0</v>
+      </c>
+      <c r="F2230">
+        <v>0</v>
+      </c>
+      <c r="G2230">
+        <v>0</v>
+      </c>
+      <c r="H2230">
+        <v>0</v>
+      </c>
+      <c r="I2230">
+        <v>8</v>
+      </c>
+      <c r="J2230">
+        <v>8</v>
+      </c>
+      <c r="K2230">
+        <v>31</v>
+      </c>
+      <c r="L2230">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2231">
+        <v>2017</v>
+      </c>
+      <c r="B2231">
+        <v>5</v>
+      </c>
+      <c r="C2231" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2231" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2231">
+        <v>0</v>
+      </c>
+      <c r="F2231">
+        <v>0</v>
+      </c>
+      <c r="G2231">
+        <v>13</v>
+      </c>
+      <c r="H2231">
+        <v>39</v>
+      </c>
+      <c r="I2231">
+        <v>0</v>
+      </c>
+      <c r="J2231">
+        <v>0</v>
+      </c>
+      <c r="K2231">
+        <v>74</v>
+      </c>
+      <c r="L2231">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2232">
+        <v>2017</v>
+      </c>
+      <c r="B2232">
+        <v>5</v>
+      </c>
+      <c r="C2232" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2232" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2232">
+        <v>3</v>
+      </c>
+      <c r="F2232">
+        <v>51</v>
+      </c>
+      <c r="G2232">
+        <v>18</v>
+      </c>
+      <c r="H2232">
+        <v>306</v>
+      </c>
+      <c r="I2232">
+        <v>-1</v>
+      </c>
+      <c r="J2232">
+        <v>-17</v>
+      </c>
+      <c r="K2232">
+        <v>14</v>
+      </c>
+      <c r="L2232">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2233">
+        <v>2017</v>
+      </c>
+      <c r="B2233">
+        <v>5</v>
+      </c>
+      <c r="C2233" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2233" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2233">
+        <v>1</v>
+      </c>
+      <c r="F2233">
+        <v>11</v>
+      </c>
+      <c r="G2233">
+        <v>4</v>
+      </c>
+      <c r="H2233">
+        <v>44</v>
+      </c>
+      <c r="I2233">
+        <v>0</v>
+      </c>
+      <c r="J2233">
+        <v>0</v>
+      </c>
+      <c r="K2233">
+        <v>2</v>
+      </c>
+      <c r="L2233">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2234">
+        <v>2017</v>
+      </c>
+      <c r="B2234">
+        <v>5</v>
+      </c>
+      <c r="C2234" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2234" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2234">
+        <v>496</v>
+      </c>
+      <c r="F2234">
+        <v>496</v>
+      </c>
+      <c r="G2234">
+        <v>8118</v>
+      </c>
+      <c r="H2234">
+        <v>8118</v>
+      </c>
+      <c r="I2234">
+        <v>0</v>
+      </c>
+      <c r="J2234">
+        <v>0</v>
+      </c>
+      <c r="K2234">
+        <v>0</v>
+      </c>
+      <c r="L2234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2235">
+        <v>2017</v>
+      </c>
+      <c r="B2235">
+        <v>5</v>
+      </c>
+      <c r="C2235" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2235" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2235">
+        <v>0</v>
+      </c>
+      <c r="F2235">
+        <v>0</v>
+      </c>
+      <c r="G2235">
+        <v>213</v>
+      </c>
+      <c r="H2235">
+        <v>639</v>
+      </c>
+      <c r="I2235">
+        <v>0</v>
+      </c>
+      <c r="J2235">
+        <v>0</v>
+      </c>
+      <c r="K2235">
+        <v>203</v>
+      </c>
+      <c r="L2235">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2236">
+        <v>2017</v>
+      </c>
+      <c r="B2236">
+        <v>5</v>
+      </c>
+      <c r="C2236" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2236" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2236">
+        <v>0</v>
+      </c>
+      <c r="F2236">
+        <v>0</v>
+      </c>
+      <c r="G2236">
+        <v>27</v>
+      </c>
+      <c r="H2236">
+        <v>459</v>
+      </c>
+      <c r="I2236">
+        <v>-2</v>
+      </c>
+      <c r="J2236">
+        <v>-34</v>
+      </c>
+      <c r="K2236">
+        <v>5</v>
+      </c>
+      <c r="L2236">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2237">
+        <v>2017</v>
+      </c>
+      <c r="B2237">
+        <v>5</v>
+      </c>
+      <c r="C2237" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2237" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2237">
+        <v>0</v>
+      </c>
+      <c r="F2237">
+        <v>0</v>
+      </c>
+      <c r="G2237">
+        <v>2</v>
+      </c>
+      <c r="H2237">
+        <v>22</v>
+      </c>
+      <c r="I2237">
+        <v>0</v>
+      </c>
+      <c r="J2237">
+        <v>0</v>
+      </c>
+      <c r="K2237">
+        <v>3</v>
+      </c>
+      <c r="L2237">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2238">
+        <v>2017</v>
+      </c>
+      <c r="B2238">
+        <v>5</v>
+      </c>
+      <c r="C2238" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2238" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2238">
+        <v>0</v>
+      </c>
+      <c r="F2238">
+        <v>0</v>
+      </c>
+      <c r="G2238">
+        <v>40</v>
+      </c>
+      <c r="H2238">
+        <v>40</v>
+      </c>
+      <c r="I2238">
+        <v>0</v>
+      </c>
+      <c r="J2238">
+        <v>0</v>
+      </c>
+      <c r="K2238">
+        <v>80</v>
+      </c>
+      <c r="L2238">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2239">
+        <v>2017</v>
+      </c>
+      <c r="B2239">
+        <v>5</v>
+      </c>
+      <c r="C2239" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2239" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2239">
+        <v>0</v>
+      </c>
+      <c r="F2239">
+        <v>0</v>
+      </c>
+      <c r="G2239">
+        <v>69</v>
+      </c>
+      <c r="H2239">
+        <v>207</v>
+      </c>
+      <c r="I2239">
+        <v>0</v>
+      </c>
+      <c r="J2239">
+        <v>0</v>
+      </c>
+      <c r="K2239">
+        <v>94</v>
+      </c>
+      <c r="L2239">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2240">
+        <v>2017</v>
+      </c>
+      <c r="B2240">
+        <v>5</v>
+      </c>
+      <c r="C2240" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2240" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2240">
+        <v>0</v>
+      </c>
+      <c r="F2240">
+        <v>0</v>
+      </c>
+      <c r="G2240">
+        <v>9</v>
+      </c>
+      <c r="H2240">
+        <v>153</v>
+      </c>
+      <c r="I2240">
+        <v>0</v>
+      </c>
+      <c r="J2240">
+        <v>0</v>
+      </c>
+      <c r="K2240">
+        <v>0</v>
+      </c>
+      <c r="L2240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2241">
+        <v>2017</v>
+      </c>
+      <c r="B2241">
+        <v>5</v>
+      </c>
+      <c r="C2241" s="1">
+        <v>220</v>
+      </c>
+      <c r="D2241" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2241">
+        <v>3</v>
+      </c>
+      <c r="F2241">
+        <v>33</v>
+      </c>
+      <c r="G2241">
+        <v>11</v>
+      </c>
+      <c r="H2241">
+        <v>121</v>
+      </c>
+      <c r="I2241">
+        <v>3</v>
+      </c>
+      <c r="J2241">
+        <v>33</v>
+      </c>
+      <c r="K2241">
+        <v>10</v>
+      </c>
+      <c r="L2241">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2242">
+        <v>2017</v>
+      </c>
+      <c r="B2242">
+        <v>5</v>
+      </c>
+      <c r="C2242" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2242" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2242">
+        <v>0</v>
+      </c>
+      <c r="F2242">
+        <v>0</v>
+      </c>
+      <c r="G2242">
+        <v>45</v>
+      </c>
+      <c r="H2242">
+        <v>45</v>
+      </c>
+      <c r="I2242">
+        <v>0</v>
+      </c>
+      <c r="J2242">
+        <v>0</v>
+      </c>
+      <c r="K2242">
+        <v>0</v>
+      </c>
+      <c r="L2242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2243">
+        <v>2017</v>
+      </c>
+      <c r="B2243">
+        <v>5</v>
+      </c>
+      <c r="C2243" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2243" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2243">
+        <v>0</v>
+      </c>
+      <c r="F2243">
+        <v>0</v>
+      </c>
+      <c r="G2243">
+        <v>184</v>
+      </c>
+      <c r="H2243">
+        <v>552</v>
+      </c>
+      <c r="I2243">
+        <v>0</v>
+      </c>
+      <c r="J2243">
+        <v>0</v>
+      </c>
+      <c r="K2243">
+        <v>93</v>
+      </c>
+      <c r="L2243">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2244">
+        <v>2017</v>
+      </c>
+      <c r="B2244">
+        <v>5</v>
+      </c>
+      <c r="C2244" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2244" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2244">
+        <v>0</v>
+      </c>
+      <c r="F2244">
+        <v>0</v>
+      </c>
+      <c r="G2244">
+        <v>11</v>
+      </c>
+      <c r="H2244">
+        <v>187</v>
+      </c>
+      <c r="I2244">
+        <v>17</v>
+      </c>
+      <c r="J2244">
+        <v>289</v>
+      </c>
+      <c r="K2244">
+        <v>73</v>
+      </c>
+      <c r="L2244">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2245">
+        <v>2017</v>
+      </c>
+      <c r="B2245">
+        <v>5</v>
+      </c>
+      <c r="C2245" s="1">
+        <v>340</v>
+      </c>
+      <c r="D2245" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2245">
+        <v>2</v>
+      </c>
+      <c r="F2245">
+        <v>22</v>
+      </c>
+      <c r="G2245">
+        <v>11</v>
+      </c>
+      <c r="H2245">
+        <v>121</v>
+      </c>
+      <c r="I2245">
+        <v>0</v>
+      </c>
+      <c r="J2245">
+        <v>0</v>
+      </c>
+      <c r="K2245">
+        <v>10</v>
+      </c>
+      <c r="L2245">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2246">
+        <v>2017</v>
+      </c>
+      <c r="B2246">
+        <v>5</v>
+      </c>
+      <c r="C2246" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2246" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2246">
+        <v>1270</v>
+      </c>
+      <c r="F2246">
+        <v>1270</v>
+      </c>
+      <c r="G2246">
+        <v>22423</v>
+      </c>
+      <c r="H2246">
+        <v>22423</v>
+      </c>
+      <c r="I2246">
+        <v>632</v>
+      </c>
+      <c r="J2246">
+        <v>632</v>
+      </c>
+      <c r="K2246">
+        <v>24296</v>
+      </c>
+      <c r="L2246">
+        <v>24296</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2247">
+        <v>2017</v>
+      </c>
+      <c r="B2247">
+        <v>5</v>
+      </c>
+      <c r="C2247" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2247" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2247">
+        <v>-3</v>
+      </c>
+      <c r="F2247">
+        <v>-9</v>
+      </c>
+      <c r="G2247">
+        <v>4501</v>
+      </c>
+      <c r="H2247">
+        <v>13503</v>
+      </c>
+      <c r="I2247">
+        <v>0</v>
+      </c>
+      <c r="J2247">
+        <v>0</v>
+      </c>
+      <c r="K2247">
+        <v>4093</v>
+      </c>
+      <c r="L2247">
+        <v>12279</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2248">
+        <v>2017</v>
+      </c>
+      <c r="B2248">
+        <v>5</v>
+      </c>
+      <c r="C2248" s="1">
+        <v>400</v>
+      </c>
+      <c r="D2248" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2248">
+        <v>-36</v>
+      </c>
+      <c r="F2248">
+        <v>-612</v>
+      </c>
+      <c r="G2248">
+        <v>1037</v>
+      </c>
+      <c r="H2248">
+        <v>17629</v>
+      </c>
+      <c r="I2248">
+        <v>-25</v>
+      </c>
+      <c r="J2248">
+        <v>-425</v>
+      </c>
+      <c r="K2248">
+        <v>742</v>
+      </c>
+      <c r="L2248">
+        <v>12614</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2249">
+        <v>2017</v>
+      </c>
+      <c r="B2249">
+        <v>5</v>
+      </c>
+      <c r="C2249" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2249" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2249">
+        <v>552</v>
+      </c>
+      <c r="F2249">
+        <v>552</v>
+      </c>
+      <c r="G2249">
+        <v>8148</v>
+      </c>
+      <c r="H2249">
+        <v>8148</v>
+      </c>
+      <c r="I2249">
+        <v>1059</v>
+      </c>
+      <c r="J2249">
+        <v>1059</v>
+      </c>
+      <c r="K2249">
+        <v>12194</v>
+      </c>
+      <c r="L2249">
+        <v>12194</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2250">
+        <v>2017</v>
+      </c>
+      <c r="B2250">
+        <v>5</v>
+      </c>
+      <c r="C2250" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2250" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2250">
+        <v>-8</v>
+      </c>
+      <c r="F2250">
+        <v>-24</v>
+      </c>
+      <c r="G2250">
+        <v>2746</v>
+      </c>
+      <c r="H2250">
+        <v>8238</v>
+      </c>
+      <c r="I2250">
+        <v>0</v>
+      </c>
+      <c r="J2250">
+        <v>0</v>
+      </c>
+      <c r="K2250">
+        <v>2720</v>
+      </c>
+      <c r="L2250">
+        <v>8160</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2251">
+        <v>2017</v>
+      </c>
+      <c r="B2251">
+        <v>5</v>
+      </c>
+      <c r="C2251" s="1">
+        <v>420</v>
+      </c>
+      <c r="D2251" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2251">
+        <v>180</v>
+      </c>
+      <c r="F2251">
+        <v>3060</v>
+      </c>
+      <c r="G2251">
+        <v>735</v>
+      </c>
+      <c r="H2251">
+        <v>12495</v>
+      </c>
+      <c r="I2251">
+        <v>297</v>
+      </c>
+      <c r="J2251">
+        <v>5049</v>
+      </c>
+      <c r="K2251">
+        <v>905</v>
+      </c>
+      <c r="L2251">
+        <v>15385</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2252">
+        <v>2017</v>
+      </c>
+      <c r="B2252">
+        <v>5</v>
+      </c>
+      <c r="C2252" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2252" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2252">
+        <v>521</v>
+      </c>
+      <c r="F2252">
+        <v>521</v>
+      </c>
+      <c r="G2252">
+        <v>9329</v>
+      </c>
+      <c r="H2252">
+        <v>9329</v>
+      </c>
+      <c r="I2252">
+        <v>360</v>
+      </c>
+      <c r="J2252">
+        <v>360</v>
+      </c>
+      <c r="K2252">
+        <v>6937</v>
+      </c>
+      <c r="L2252">
+        <v>6937</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2253">
+        <v>2017</v>
+      </c>
+      <c r="B2253">
+        <v>5</v>
+      </c>
+      <c r="C2253" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2253" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2253">
+        <v>0</v>
+      </c>
+      <c r="F2253">
+        <v>0</v>
+      </c>
+      <c r="G2253">
+        <v>1183</v>
+      </c>
+      <c r="H2253">
+        <v>3549</v>
+      </c>
+      <c r="I2253">
+        <v>0</v>
+      </c>
+      <c r="J2253">
+        <v>0</v>
+      </c>
+      <c r="K2253">
+        <v>917</v>
+      </c>
+      <c r="L2253">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2254">
+        <v>2017</v>
+      </c>
+      <c r="B2254">
+        <v>5</v>
+      </c>
+      <c r="C2254" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2254" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2254">
+        <v>44</v>
+      </c>
+      <c r="F2254">
+        <v>748</v>
+      </c>
+      <c r="G2254">
+        <v>1371</v>
+      </c>
+      <c r="H2254">
+        <v>23307</v>
+      </c>
+      <c r="I2254">
+        <v>152</v>
+      </c>
+      <c r="J2254">
+        <v>2584</v>
+      </c>
+      <c r="K2254">
+        <v>1453</v>
+      </c>
+      <c r="L2254">
+        <v>24701</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2255">
+        <v>2017</v>
+      </c>
+      <c r="B2255">
+        <v>5</v>
+      </c>
+      <c r="C2255" s="1">
+        <v>540</v>
+      </c>
+      <c r="D2255" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2255">
+        <v>1</v>
+      </c>
+      <c r="F2255">
+        <v>11</v>
+      </c>
+      <c r="G2255">
+        <v>9</v>
+      </c>
+      <c r="H2255">
+        <v>99</v>
+      </c>
+      <c r="I2255">
+        <v>6</v>
+      </c>
+      <c r="J2255">
+        <v>66</v>
+      </c>
+      <c r="K2255">
+        <v>15</v>
+      </c>
+      <c r="L2255">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2256">
+        <v>2017</v>
+      </c>
+      <c r="B2256">
+        <v>5</v>
+      </c>
+      <c r="C2256" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2256" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2256">
+        <v>10</v>
+      </c>
+      <c r="F2256">
+        <v>10</v>
+      </c>
+      <c r="G2256">
+        <v>9955</v>
+      </c>
+      <c r="H2256">
+        <v>9955</v>
+      </c>
+      <c r="I2256">
+        <v>78</v>
+      </c>
+      <c r="J2256">
+        <v>78</v>
+      </c>
+      <c r="K2256">
+        <v>10424</v>
+      </c>
+      <c r="L2256">
+        <v>10424</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2257">
+        <v>2017</v>
+      </c>
+      <c r="B2257">
+        <v>5</v>
+      </c>
+      <c r="C2257" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2257" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2257">
+        <v>0</v>
+      </c>
+      <c r="F2257">
+        <v>0</v>
+      </c>
+      <c r="G2257">
+        <v>2139</v>
+      </c>
+      <c r="H2257">
+        <v>6417</v>
+      </c>
+      <c r="I2257">
+        <v>-14</v>
+      </c>
+      <c r="J2257">
+        <v>-42</v>
+      </c>
+      <c r="K2257">
+        <v>1876</v>
+      </c>
+      <c r="L2257">
+        <v>5628</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2258">
+        <v>2017</v>
+      </c>
+      <c r="B2258">
+        <v>5</v>
+      </c>
+      <c r="C2258" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2258" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2258">
+        <v>0</v>
+      </c>
+      <c r="F2258">
+        <v>0</v>
+      </c>
+      <c r="G2258">
+        <v>126</v>
+      </c>
+      <c r="H2258">
+        <v>2142</v>
+      </c>
+      <c r="I2258">
+        <v>41</v>
+      </c>
+      <c r="J2258">
+        <v>697</v>
+      </c>
+      <c r="K2258">
+        <v>175</v>
+      </c>
+      <c r="L2258">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2259">
+        <v>2017</v>
+      </c>
+      <c r="B2259">
+        <v>5</v>
+      </c>
+      <c r="C2259" s="1">
+        <v>575</v>
+      </c>
+      <c r="D2259" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2259">
+        <v>4</v>
+      </c>
+      <c r="F2259">
+        <v>47</v>
+      </c>
+      <c r="G2259">
+        <v>32</v>
+      </c>
+      <c r="H2259">
+        <v>354</v>
+      </c>
+      <c r="I2259">
+        <v>2</v>
+      </c>
+      <c r="J2259">
+        <v>25</v>
+      </c>
+      <c r="K2259">
+        <v>26</v>
+      </c>
+      <c r="L2259">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2260">
+        <v>2017</v>
+      </c>
+      <c r="B2260">
+        <v>5</v>
+      </c>
+      <c r="C2260" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2260" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2260">
+        <v>0</v>
+      </c>
+      <c r="F2260">
+        <v>0</v>
+      </c>
+      <c r="G2260">
+        <v>140</v>
+      </c>
+      <c r="H2260">
+        <v>140</v>
+      </c>
+      <c r="I2260">
+        <v>0</v>
+      </c>
+      <c r="J2260">
+        <v>0</v>
+      </c>
+      <c r="K2260">
+        <v>0</v>
+      </c>
+      <c r="L2260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2261">
+        <v>2017</v>
+      </c>
+      <c r="B2261">
+        <v>5</v>
+      </c>
+      <c r="C2261" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2261" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2261">
+        <v>0</v>
+      </c>
+      <c r="F2261">
+        <v>0</v>
+      </c>
+      <c r="G2261">
+        <v>4</v>
+      </c>
+      <c r="H2261">
+        <v>12</v>
+      </c>
+      <c r="I2261">
+        <v>0</v>
+      </c>
+      <c r="J2261">
+        <v>0</v>
+      </c>
+      <c r="K2261">
+        <v>1</v>
+      </c>
+      <c r="L2261">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2262">
+        <v>2017</v>
+      </c>
+      <c r="B2262">
+        <v>5</v>
+      </c>
+      <c r="C2262" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2262" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2262">
+        <v>0</v>
+      </c>
+      <c r="F2262">
+        <v>0</v>
+      </c>
+      <c r="G2262">
+        <v>-1</v>
+      </c>
+      <c r="H2262">
+        <v>-17</v>
+      </c>
+      <c r="I2262">
+        <v>26</v>
+      </c>
+      <c r="J2262">
+        <v>442</v>
+      </c>
+      <c r="K2262">
+        <v>26</v>
+      </c>
+      <c r="L2262">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2263">
+        <v>2017</v>
+      </c>
+      <c r="B2263">
+        <v>5</v>
+      </c>
+      <c r="C2263" s="1">
+        <v>640</v>
+      </c>
+      <c r="D2263" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2263">
+        <v>1</v>
+      </c>
+      <c r="F2263">
+        <v>11</v>
+      </c>
+      <c r="G2263">
+        <v>7</v>
+      </c>
+      <c r="H2263">
+        <v>77</v>
+      </c>
+      <c r="I2263">
+        <v>1</v>
+      </c>
+      <c r="J2263">
+        <v>11</v>
+      </c>
+      <c r="K2263">
+        <v>5</v>
+      </c>
+      <c r="L2263">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2264">
+        <v>2017</v>
+      </c>
+      <c r="B2264">
+        <v>5</v>
+      </c>
+      <c r="C2264" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2264" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2264">
+        <v>12</v>
+      </c>
+      <c r="F2264">
+        <v>12</v>
+      </c>
+      <c r="G2264">
+        <v>222</v>
+      </c>
+      <c r="H2264">
+        <v>222</v>
+      </c>
+      <c r="I2264">
+        <v>-44</v>
+      </c>
+      <c r="J2264">
+        <v>-44</v>
+      </c>
+      <c r="K2264">
+        <v>150</v>
+      </c>
+      <c r="L2264">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2265">
+        <v>2017</v>
+      </c>
+      <c r="B2265">
+        <v>5</v>
+      </c>
+      <c r="C2265" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2265" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2265">
+        <v>0</v>
+      </c>
+      <c r="F2265">
+        <v>0</v>
+      </c>
+      <c r="G2265">
+        <v>209</v>
+      </c>
+      <c r="H2265">
+        <v>627</v>
+      </c>
+      <c r="I2265">
+        <v>0</v>
+      </c>
+      <c r="J2265">
+        <v>0</v>
+      </c>
+      <c r="K2265">
+        <v>272</v>
+      </c>
+      <c r="L2265">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2266">
+        <v>2017</v>
+      </c>
+      <c r="B2266">
+        <v>5</v>
+      </c>
+      <c r="C2266" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2266" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2266">
+        <v>7</v>
+      </c>
+      <c r="F2266">
+        <v>135</v>
+      </c>
+      <c r="G2266">
+        <v>56</v>
+      </c>
+      <c r="H2266">
+        <v>968</v>
+      </c>
+      <c r="I2266">
+        <v>29</v>
+      </c>
+      <c r="J2266">
+        <v>493</v>
+      </c>
+      <c r="K2266">
+        <v>42</v>
+      </c>
+      <c r="L2266">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2267">
+        <v>2017</v>
+      </c>
+      <c r="B2267">
+        <v>5</v>
+      </c>
+      <c r="C2267" s="1">
+        <v>685</v>
+      </c>
+      <c r="D2267" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2267">
+        <v>0</v>
+      </c>
+      <c r="F2267">
+        <v>0</v>
+      </c>
+      <c r="G2267">
+        <v>2</v>
+      </c>
+      <c r="H2267">
+        <v>22</v>
+      </c>
+      <c r="I2267">
+        <v>0</v>
+      </c>
+      <c r="J2267">
+        <v>0</v>
+      </c>
+      <c r="K2267">
+        <v>4</v>
+      </c>
+      <c r="L2267">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2268">
+        <v>2017</v>
+      </c>
+      <c r="B2268">
+        <v>5</v>
+      </c>
+      <c r="C2268" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2268" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2268">
+        <v>0</v>
+      </c>
+      <c r="F2268">
+        <v>0</v>
+      </c>
+      <c r="G2268">
+        <v>0</v>
+      </c>
+      <c r="H2268">
+        <v>0</v>
+      </c>
+      <c r="I2268">
+        <v>0</v>
+      </c>
+      <c r="J2268">
+        <v>0</v>
+      </c>
+      <c r="K2268">
+        <v>54</v>
+      </c>
+      <c r="L2268">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2269">
+        <v>2017</v>
+      </c>
+      <c r="B2269">
+        <v>5</v>
+      </c>
+      <c r="C2269" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2269" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2269">
+        <v>-13</v>
+      </c>
+      <c r="F2269">
+        <v>-41</v>
+      </c>
+      <c r="G2269">
+        <v>485</v>
+      </c>
+      <c r="H2269">
+        <v>1455</v>
+      </c>
+      <c r="I2269">
+        <v>0</v>
+      </c>
+      <c r="J2269">
+        <v>0</v>
+      </c>
+      <c r="K2269">
+        <v>208</v>
+      </c>
+      <c r="L2269">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2270">
+        <v>2017</v>
+      </c>
+      <c r="B2270">
+        <v>5</v>
+      </c>
+      <c r="C2270" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2270" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2270">
+        <v>-3</v>
+      </c>
+      <c r="F2270">
+        <v>-51</v>
+      </c>
+      <c r="G2270">
+        <v>14</v>
+      </c>
+      <c r="H2270">
+        <v>238</v>
+      </c>
+      <c r="I2270">
+        <v>14</v>
+      </c>
+      <c r="J2270">
+        <v>238</v>
+      </c>
+      <c r="K2270">
+        <v>60</v>
+      </c>
+      <c r="L2270">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2271">
+        <v>2017</v>
+      </c>
+      <c r="B2271">
+        <v>5</v>
+      </c>
+      <c r="C2271" s="1">
+        <v>700</v>
+      </c>
+      <c r="D2271" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2271">
+        <v>1</v>
+      </c>
+      <c r="F2271">
+        <v>11</v>
+      </c>
+      <c r="G2271">
+        <v>9</v>
+      </c>
+      <c r="H2271">
+        <v>99</v>
+      </c>
+      <c r="I2271">
+        <v>0</v>
+      </c>
+      <c r="J2271">
+        <v>0</v>
+      </c>
+      <c r="K2271">
+        <v>8</v>
+      </c>
+      <c r="L2271">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2272">
+        <v>2017</v>
+      </c>
+      <c r="B2272">
+        <v>5</v>
+      </c>
+      <c r="C2272" s="1">
+        <v>820</v>
+      </c>
+      <c r="D2272" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2272">
+        <v>1</v>
+      </c>
+      <c r="F2272">
+        <v>11</v>
+      </c>
+      <c r="G2272">
+        <v>4</v>
+      </c>
+      <c r="H2272">
+        <v>44</v>
+      </c>
+      <c r="I2272">
+        <v>0</v>
+      </c>
+      <c r="J2272">
+        <v>0</v>
+      </c>
+      <c r="K2272">
+        <v>5</v>
+      </c>
+      <c r="L2272">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2273">
+        <v>2017</v>
+      </c>
+      <c r="B2273">
+        <v>5</v>
+      </c>
+      <c r="C2273" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2273" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2273">
+        <v>335</v>
+      </c>
+      <c r="F2273">
+        <v>335</v>
+      </c>
+      <c r="G2273">
+        <v>15841</v>
+      </c>
+      <c r="H2273">
+        <v>15841</v>
+      </c>
+      <c r="I2273">
+        <v>897</v>
+      </c>
+      <c r="J2273">
+        <v>897</v>
+      </c>
+      <c r="K2273">
+        <v>17874</v>
+      </c>
+      <c r="L2273">
+        <v>17874</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2274">
+        <v>2017</v>
+      </c>
+      <c r="B2274">
+        <v>5</v>
+      </c>
+      <c r="C2274" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2274" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2274">
+        <v>13</v>
+      </c>
+      <c r="F2274">
+        <v>41</v>
+      </c>
+      <c r="G2274">
+        <v>3330</v>
+      </c>
+      <c r="H2274">
+        <v>9992</v>
+      </c>
+      <c r="I2274">
+        <v>-2</v>
+      </c>
+      <c r="J2274">
+        <v>-6</v>
+      </c>
+      <c r="K2274">
+        <v>2305</v>
+      </c>
+      <c r="L2274">
+        <v>6915</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2275">
+        <v>2017</v>
+      </c>
+      <c r="B2275">
+        <v>5</v>
+      </c>
+      <c r="C2275" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2275" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2275">
+        <v>4</v>
+      </c>
+      <c r="F2275">
+        <v>68</v>
+      </c>
+      <c r="G2275">
+        <v>305</v>
+      </c>
+      <c r="H2275">
+        <v>5185</v>
+      </c>
+      <c r="I2275">
+        <v>32</v>
+      </c>
+      <c r="J2275">
+        <v>544</v>
+      </c>
+      <c r="K2275">
+        <v>448</v>
+      </c>
+      <c r="L2275">
+        <v>7616</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2276">
+        <v>2017</v>
+      </c>
+      <c r="B2276">
+        <v>5</v>
+      </c>
+      <c r="C2276" s="1">
+        <v>840</v>
+      </c>
+      <c r="D2276" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2276">
+        <v>0</v>
+      </c>
+      <c r="F2276">
+        <v>0</v>
+      </c>
+      <c r="G2276">
+        <v>2</v>
+      </c>
+      <c r="H2276">
+        <v>22</v>
+      </c>
+      <c r="I2276">
+        <v>0</v>
+      </c>
+      <c r="J2276">
+        <v>0</v>
+      </c>
+      <c r="K2276">
+        <v>0</v>
+      </c>
+      <c r="L2276">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>